<commit_message>
We got cstar back
</commit_message>
<xml_diff>
--- a/REGEN/Contour_Maelstrom.xlsx
+++ b/REGEN/Contour_Maelstrom.xlsx
@@ -59,7 +59,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="true"/>
+    <col min="1" max="1" width="14.5546875" customWidth="true"/>
     <col min="2" max="2" width="13.5546875" customWidth="true"/>
     <col min="3" max="3" width="11.5546875" customWidth="true"/>
   </cols>
@@ -72,2746 +72,2746 @@
         <v>0.043179999999999996</v>
       </c>
       <c r="C1" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.00061204819277108427</v>
+        <v>0.0010302811244979919</v>
       </c>
       <c r="B2" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C2" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.0012240963855421685</v>
+        <v>0.0020605622489959837</v>
       </c>
       <c r="B3" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C3" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.0018361445783132528</v>
+        <v>0.003090843373493976</v>
       </c>
       <c r="B4" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C4" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.0024481927710843371</v>
+        <v>0.0041211244979919674</v>
       </c>
       <c r="B5" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C5" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.0030602409638554214</v>
+        <v>0.0051514056224899593</v>
       </c>
       <c r="B6" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C6" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.0036722891566265056</v>
+        <v>0.006181686746987952</v>
       </c>
       <c r="B7" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C7" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.004284337349397589</v>
+        <v>0.0072119678714859439</v>
       </c>
       <c r="B8" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C8" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.0048963855421686742</v>
+        <v>0.0082422489959839348</v>
       </c>
       <c r="B9" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C9" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.0055084337349397584</v>
+        <v>0.0092725301204819276</v>
       </c>
       <c r="B10" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C10" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.0061204819277108427</v>
+        <v>0.010302811244979919</v>
       </c>
       <c r="B11" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C11" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.0067325301204819261</v>
+        <v>0.01133309236947791</v>
       </c>
       <c r="B12" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C12" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.0073445783132530112</v>
+        <v>0.012363373493975904</v>
       </c>
       <c r="B13" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C13" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.0079566265060240955</v>
+        <v>0.013393654618473897</v>
       </c>
       <c r="B14" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C14" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.0085686746987951781</v>
+        <v>0.014423935742971888</v>
       </c>
       <c r="B15" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C15" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.0091807228915662641</v>
+        <v>0.015454216867469879</v>
       </c>
       <c r="B16" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C16" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.0097927710843373483</v>
+        <v>0.01648449799196787</v>
       </c>
       <c r="B17" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C17" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.010404819277108433</v>
+        <v>0.017514779116465862</v>
       </c>
       <c r="B18" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C18" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.011016867469879517</v>
+        <v>0.018545060240963855</v>
       </c>
       <c r="B19" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C19" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.011628915662650601</v>
+        <v>0.019575341365461844</v>
       </c>
       <c r="B20" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C20" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.012240963855421685</v>
+        <v>0.020605622489959837</v>
       </c>
       <c r="B21" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C21" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.01285301204819277</v>
+        <v>0.02163590361445783</v>
       </c>
       <c r="B22" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C22" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.013465060240963852</v>
+        <v>0.022666184738955819</v>
       </c>
       <c r="B23" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C23" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.014077108433734938</v>
+        <v>0.023696465863453812</v>
       </c>
       <c r="B24" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C24" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.014689156626506022</v>
+        <v>0.024726746987951808</v>
       </c>
       <c r="B25" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C25" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.015301204819277107</v>
+        <v>0.025757028112449801</v>
       </c>
       <c r="B26" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C26" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.015913253012048191</v>
+        <v>0.026787309236947793</v>
       </c>
       <c r="B27" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C27" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.016525301204819275</v>
+        <v>0.027817590361445783</v>
       </c>
       <c r="B28" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C28" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.017137349397590356</v>
+        <v>0.028847871485943776</v>
       </c>
       <c r="B29" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C29" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.01774939759036144</v>
+        <v>0.029878152610441768</v>
       </c>
       <c r="B30" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C30" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.018361445783132528</v>
+        <v>0.030908433734939757</v>
       </c>
       <c r="B31" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C31" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.018973493975903612</v>
+        <v>0.03193871485943775</v>
       </c>
       <c r="B32" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C32" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.019585542168674697</v>
+        <v>0.032968995983935739</v>
       </c>
       <c r="B33" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C33" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.020197590361445781</v>
+        <v>0.033999277108433729</v>
       </c>
       <c r="B34" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C34" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.020809638554216865</v>
+        <v>0.035029558232931725</v>
       </c>
       <c r="B35" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C35" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.021421686746987949</v>
+        <v>0.036059839357429714</v>
       </c>
       <c r="B36" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C36" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.022033734939759034</v>
+        <v>0.03709012048192771</v>
       </c>
       <c r="B37" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C37" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.022645783132530115</v>
+        <v>0.0381204016064257</v>
       </c>
       <c r="B38" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C38" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.023257831325301202</v>
+        <v>0.039150682730923689</v>
       </c>
       <c r="B39" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C39" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.023869879518072287</v>
+        <v>0.040180963855421685</v>
       </c>
       <c r="B40" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C40" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.024481927710843371</v>
+        <v>0.041211244979919674</v>
       </c>
       <c r="B41" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C41" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.025093975903614455</v>
+        <v>0.042241526104417664</v>
       </c>
       <c r="B42" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C42" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.025706024096385539</v>
+        <v>0.04327180722891566</v>
       </c>
       <c r="B43" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C43" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.026318072289156624</v>
+        <v>0.044302088353413649</v>
       </c>
       <c r="B44" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C44" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.026930120481927705</v>
+        <v>0.045332369477911638</v>
       </c>
       <c r="B45" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C45" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.027542168674698789</v>
+        <v>0.046362650602409634</v>
       </c>
       <c r="B46" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C46" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.028154216867469876</v>
+        <v>0.047392931726907624</v>
       </c>
       <c r="B47" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C47" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.028766265060240961</v>
+        <v>0.048423212851405627</v>
       </c>
       <c r="B48" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C48" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.029378313253012045</v>
+        <v>0.049453493975903616</v>
       </c>
       <c r="B49" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C49" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.029990361445783129</v>
+        <v>0.050483775100401605</v>
       </c>
       <c r="B50" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C50" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.030602409638554214</v>
+        <v>0.051514056224899602</v>
       </c>
       <c r="B51" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C51" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.031214457831325298</v>
+        <v>0.052544337349397591</v>
       </c>
       <c r="B52" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C52" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.031826506024096382</v>
+        <v>0.053574618473895587</v>
       </c>
       <c r="B53" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.03243855421686747</v>
+        <v>0.054604899598393576</v>
       </c>
       <c r="B54" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C54" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.033050602409638551</v>
+        <v>0.055635180722891565</v>
       </c>
       <c r="B55" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.033662650602409638</v>
+        <v>0.056665461847389562</v>
       </c>
       <c r="B56" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C56" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.034274698795180712</v>
+        <v>0.057695742971887551</v>
       </c>
       <c r="B57" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C57" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.0348867469879518</v>
+        <v>0.05872602409638554</v>
       </c>
       <c r="B58" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C58" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.035498795180722881</v>
+        <v>0.059756305220883536</v>
       </c>
       <c r="B59" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.036110843373493969</v>
+        <v>0.060786586345381526</v>
       </c>
       <c r="B60" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C60" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.036722891566265056</v>
+        <v>0.061816867469879515</v>
       </c>
       <c r="B61" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C61" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0.037334939759036137</v>
+        <v>0.062847148594377511</v>
       </c>
       <c r="B62" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C62" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.037946987951807225</v>
+        <v>0.0638774297188755</v>
       </c>
       <c r="B63" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C63" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.038559036144578306</v>
+        <v>0.06490771084337349</v>
       </c>
       <c r="B64" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C64" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0.039171084337349393</v>
+        <v>0.065937991967871479</v>
       </c>
       <c r="B65" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C65" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.039783132530120474</v>
+        <v>0.066968273092369482</v>
       </c>
       <c r="B66" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C66" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.040395180722891562</v>
+        <v>0.067998554216867457</v>
       </c>
       <c r="B67" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C67" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0.04100722891566265</v>
+        <v>0.06902883534136546</v>
       </c>
       <c r="B68" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C68" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.04161927710843373</v>
+        <v>0.07005911646586345</v>
       </c>
       <c r="B69" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C69" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.042231325301204818</v>
+        <v>0.071089397590361439</v>
       </c>
       <c r="B70" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C70" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0.042843373493975899</v>
+        <v>0.072119678714859428</v>
       </c>
       <c r="B71" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C71" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.043455421686746987</v>
+        <v>0.073149959839357431</v>
       </c>
       <c r="B72" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C72" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.044067469879518067</v>
+        <v>0.074180240963855421</v>
       </c>
       <c r="B73" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C73" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0.044679518072289148</v>
+        <v>0.07521052208835341</v>
       </c>
       <c r="B74" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C74" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.045291566265060229</v>
+        <v>0.076240803212851399</v>
       </c>
       <c r="B75" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C75" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.045903614457831317</v>
+        <v>0.077271084337349402</v>
       </c>
       <c r="B76" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C76" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0.046515662650602405</v>
+        <v>0.078301365461847378</v>
       </c>
       <c r="B77" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C77" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.047127710843373485</v>
+        <v>0.079331646586345381</v>
       </c>
       <c r="B78" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C78" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.047739759036144573</v>
+        <v>0.08036192771084337</v>
       </c>
       <c r="B79" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C79" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0.048351807228915654</v>
+        <v>0.081392208835341359</v>
       </c>
       <c r="B80" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C80" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.048963855421686742</v>
+        <v>0.082422489959839348</v>
       </c>
       <c r="B81" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C81" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.049575903614457823</v>
+        <v>0.083452771084337352</v>
       </c>
       <c r="B82" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C82" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.05018795180722891</v>
+        <v>0.084483052208835327</v>
       </c>
       <c r="B83" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C83" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.050799999999999998</v>
+        <v>0.08551333333333333</v>
       </c>
       <c r="B84" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C84" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.051412048192771079</v>
+        <v>0.086543614457831319</v>
       </c>
       <c r="B85" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C85" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.052024096385542167</v>
+        <v>0.087573895582329309</v>
       </c>
       <c r="B86" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C86" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.052636144578313247</v>
+        <v>0.088604176706827298</v>
       </c>
       <c r="B87" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C87" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.053248192771084335</v>
+        <v>0.089634457831325301</v>
       </c>
       <c r="B88" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C88" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.053860240963855409</v>
+        <v>0.090664738955823276</v>
       </c>
       <c r="B89" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C89" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.054472289156626497</v>
+        <v>0.09169502008032128</v>
       </c>
       <c r="B90" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C90" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.055084337349397577</v>
+        <v>0.092725301204819269</v>
       </c>
       <c r="B91" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C91" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>0.055696385542168665</v>
+        <v>0.093755582329317272</v>
       </c>
       <c r="B92" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C92" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>0.056308433734939753</v>
+        <v>0.094785863453815247</v>
       </c>
       <c r="B93" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C93" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.056920481927710834</v>
+        <v>0.09581614457831325</v>
       </c>
       <c r="B94" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C94" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>0.057532530120481921</v>
+        <v>0.096846425702811254</v>
       </c>
       <c r="B95" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C95" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>0.058144578313253002</v>
+        <v>0.097876706827309229</v>
       </c>
       <c r="B96" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C96" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.05875662650602409</v>
+        <v>0.098906987951807232</v>
       </c>
       <c r="B97" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C97" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>0.059368674698795171</v>
+        <v>0.099937269076305221</v>
       </c>
       <c r="B98" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C98" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>0.059980722891566259</v>
+        <v>0.10096755020080321</v>
       </c>
       <c r="B99" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C99" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.060592771084337339</v>
+        <v>0.1019978313253012</v>
       </c>
       <c r="B100" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C100" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>0.061204819277108427</v>
+        <v>0.1030281124497992</v>
       </c>
       <c r="B101" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C101" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>0.061816867469879515</v>
+        <v>0.10405839357429718</v>
       </c>
       <c r="B102" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C102" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.062428915662650596</v>
+        <v>0.10508867469879518</v>
       </c>
       <c r="B103" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C103" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0">
-        <v>0.063040963855421683</v>
+        <v>0.10611895582329317</v>
       </c>
       <c r="B104" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C104" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.063653012048192764</v>
+        <v>0.10714923694779117</v>
       </c>
       <c r="B105" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C105" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.064265060240963845</v>
+        <v>0.10817951807228915</v>
       </c>
       <c r="B106" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C106" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>0.06487710843373494</v>
+        <v>0.10920979919678715</v>
       </c>
       <c r="B107" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C107" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.065489156626506021</v>
+        <v>0.11024008032128514</v>
       </c>
       <c r="B108" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C108" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.066101204819277101</v>
+        <v>0.11127036144578313</v>
       </c>
       <c r="B109" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C109" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>0.066713253012048196</v>
+        <v>0.11230064257028112</v>
       </c>
       <c r="B110" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C110" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.067325301204819277</v>
+        <v>0.11333092369477912</v>
       </c>
       <c r="B111" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C111" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.067937349397590358</v>
+        <v>0.1143612048192771</v>
       </c>
       <c r="B112" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C112" s="0">
-        <v>8.2732603946705385</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>0.068549397590361424</v>
+        <v>0.1153914859437751</v>
       </c>
       <c r="B113" s="0">
-        <v>0.043172720429257364</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C113" s="0">
-        <v>8.2704711076078183</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.069161445783132519</v>
+        <v>0.11642176706827309</v>
       </c>
       <c r="B114" s="0">
-        <v>0.04313718220341712</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C114" s="0">
-        <v>8.2568608048141545</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.0697734939759036</v>
+        <v>0.11745204819277108</v>
       </c>
       <c r="B115" s="0">
-        <v>0.043071829286690719</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C115" s="0">
-        <v>8.2318614351755457</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>0.070385542168674681</v>
+        <v>0.11848232931726907</v>
       </c>
       <c r="B116" s="0">
-        <v>0.042976193910918496</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C116" s="0">
-        <v>8.1953464705785688</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.070997590361445762</v>
+        <v>0.11951261044176707</v>
       </c>
       <c r="B117" s="0">
-        <v>0.042849573709422738</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C117" s="0">
-        <v>8.1471259256023902</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.071609638554216856</v>
+        <v>0.12054289156626505</v>
       </c>
       <c r="B118" s="0">
-        <v>0.042691004842594201</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C118" s="0">
-        <v>8.086939088172274</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>0.072221686746987937</v>
+        <v>0.12157317269076305</v>
       </c>
       <c r="B119" s="0">
-        <v>0.042499222886623223</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C119" s="0">
-        <v>8.0144439402266983</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.072833734939759018</v>
+        <v>0.12260345381526104</v>
       </c>
       <c r="B120" s="0">
-        <v>0.042272607529730097</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C120" s="0">
-        <v>7.9292021984229173</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.073445783132530112</v>
+        <v>0.12363373493975903</v>
       </c>
       <c r="B121" s="0">
-        <v>0.042009104905482375</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C121" s="0">
-        <v>7.8306583058262449</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0">
-        <v>0.074057831325301193</v>
+        <v>0.12466401606425702</v>
       </c>
       <c r="B122" s="0">
-        <v>0.041706117829082318</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C122" s="0">
-        <v>7.7181097415705446</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>0.074669879518072274</v>
+        <v>0.12569429718875502</v>
       </c>
       <c r="B123" s="0">
-        <v>0.041360348207787903</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C123" s="0">
-        <v>7.5906643939463487</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.075281927710843355</v>
+        <v>0.12672457831325301</v>
       </c>
       <c r="B124" s="0">
-        <v>0.040967565339602816</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C124" s="0">
-        <v>7.4471778867685705</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0">
-        <v>0.07589397590361445</v>
+        <v>0.127754859437751</v>
       </c>
       <c r="B125" s="0">
-        <v>0.04052225424900277</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C125" s="0">
-        <v>7.2861584565764748</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>0.07650602409638553</v>
+        <v>0.12878514056224899</v>
       </c>
       <c r="B126" s="0">
-        <v>0.040017059718290622</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C126" s="0">
-        <v>7.1056165668874485</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.077118072289156611</v>
+        <v>0.12981542168674698</v>
       </c>
       <c r="B127" s="0">
-        <v>0.039441897890935135</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C127" s="0">
-        <v>6.9028275938356565</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0">
-        <v>0.077730120481927706</v>
+        <v>0.13084570281124497</v>
       </c>
       <c r="B128" s="0">
-        <v>0.03882984969816404</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C128" s="0">
-        <v>6.6902575470844274</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>0.078342168674698787</v>
+        <v>0.13187598393574296</v>
       </c>
       <c r="B129" s="0">
-        <v>0.038217801505392959</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C129" s="0">
-        <v>6.4810118955833129</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.078954216867469867</v>
+        <v>0.13290626506024098</v>
       </c>
       <c r="B130" s="0">
-        <v>0.037605753312621879</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C130" s="0">
-        <v>6.2750906393323014</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0">
-        <v>0.079566265060240948</v>
+        <v>0.13393654618473896</v>
       </c>
       <c r="B131" s="0">
-        <v>0.036993705119850798</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C131" s="0">
-        <v>6.0724937783313981</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.080178313253012043</v>
+        <v>0.13496682730923695</v>
       </c>
       <c r="B132" s="0">
-        <v>0.036381656927079703</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C132" s="0">
-        <v>5.8732213125805943</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.080790361445783124</v>
+        <v>0.13599710843373491</v>
       </c>
       <c r="B133" s="0">
-        <v>0.035769608734308622</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C133" s="0">
-        <v>5.6772732420799033</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0">
-        <v>0.081402409638554205</v>
+        <v>0.13702738955823293</v>
       </c>
       <c r="B134" s="0">
-        <v>0.035157560541537541</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C134" s="0">
-        <v>5.484649566829316</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.082014457831325299</v>
+        <v>0.13805767068273092</v>
       </c>
       <c r="B135" s="0">
-        <v>0.034545512348766447</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C135" s="0">
-        <v>5.2953502868288327</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.08262650602409638</v>
+        <v>0.13908795180722891</v>
       </c>
       <c r="B136" s="0">
-        <v>0.033933464155995366</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C136" s="0">
-        <v>5.1093754020784576</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0">
-        <v>0.083238554216867461</v>
+        <v>0.1401182329317269</v>
       </c>
       <c r="B137" s="0">
-        <v>0.033321415963224292</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C137" s="0">
-        <v>4.9267249125781927</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.083850602409638542</v>
+        <v>0.14114851405622492</v>
       </c>
       <c r="B138" s="0">
-        <v>0.032709367770453211</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C138" s="0">
-        <v>4.7473988183280289</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.084462650602409636</v>
+        <v>0.14217879518072288</v>
       </c>
       <c r="B139" s="0">
-        <v>0.032097319577682117</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C139" s="0">
-        <v>4.5713971193279708</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0">
-        <v>0.085074698795180717</v>
+        <v>0.14320907630522087</v>
       </c>
       <c r="B140" s="0">
-        <v>0.031485271384911036</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C140" s="0">
-        <v>4.3987198155780201</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.085686746987951798</v>
+        <v>0.14423935742971886</v>
       </c>
       <c r="B141" s="0">
-        <v>0.030873223192139955</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C141" s="0">
-        <v>4.2293669070781768</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.086298795180722893</v>
+        <v>0.14526963855421687</v>
       </c>
       <c r="B142" s="0">
-        <v>0.03026117499936886</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C142" s="0">
-        <v>4.0633383938284346</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0">
-        <v>0.086910843373493973</v>
+        <v>0.14629991967871486</v>
       </c>
       <c r="B143" s="0">
-        <v>0.029649126806597779</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C143" s="0">
-        <v>3.9006342758288026</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.087522891566265054</v>
+        <v>0.14733020080321285</v>
       </c>
       <c r="B144" s="0">
-        <v>0.029037078613826699</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C144" s="0">
-        <v>3.7412545530792771</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.088134939759036135</v>
+        <v>0.14836048192771084</v>
       </c>
       <c r="B145" s="0">
-        <v>0.028425030421055618</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C145" s="0">
-        <v>3.5851992255798577</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0">
-        <v>0.088746987951807216</v>
+        <v>0.14939076305220883</v>
       </c>
       <c r="B146" s="0">
-        <v>0.027812982228284537</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C146" s="0">
-        <v>3.4324682933305439</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>0.089359036144578297</v>
+        <v>0.15042104417670682</v>
       </c>
       <c r="B147" s="0">
-        <v>0.027200934035513456</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C147" s="0">
-        <v>3.2830617563313367</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.089971084337349377</v>
+        <v>0.15145132530120481</v>
       </c>
       <c r="B148" s="0">
-        <v>0.026588885842742375</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C148" s="0">
-        <v>3.1369796145822351</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0">
-        <v>0.090583132530120458</v>
+        <v>0.1524816064257028</v>
       </c>
       <c r="B149" s="0">
-        <v>0.025976837649971295</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C149" s="0">
-        <v>2.9942218680832395</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>0.091195180722891553</v>
+        <v>0.15351188755020082</v>
       </c>
       <c r="B150" s="0">
-        <v>0.0253647894572002</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C150" s="0">
-        <v>2.854788516834347</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.091807228915662634</v>
+        <v>0.15454216867469881</v>
       </c>
       <c r="B151" s="0">
-        <v>0.024752741264429119</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C151" s="0">
-        <v>2.7186795608355636</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0">
-        <v>0.092419277108433715</v>
+        <v>0.15557244979919677</v>
       </c>
       <c r="B152" s="0">
-        <v>0.024140693071658038</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C152" s="0">
-        <v>2.5858950000868863</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>0.093031325301204809</v>
+        <v>0.15660273092369476</v>
       </c>
       <c r="B153" s="0">
-        <v>0.023528644878886944</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C153" s="0">
-        <v>2.4564348345883125</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0">
-        <v>0.09364337349397589</v>
+        <v>0.15763301204819277</v>
       </c>
       <c r="B154" s="0">
-        <v>0.022916596686115863</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C154" s="0">
-        <v>2.3302990643398474</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0">
-        <v>0.094255421686746971</v>
+        <v>0.15866329317269076</v>
       </c>
       <c r="B155" s="0">
-        <v>0.022304548493344782</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C155" s="0">
-        <v>2.2074876893414883</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0">
-        <v>0.094867469879518052</v>
+        <v>0.15969357429718875</v>
       </c>
       <c r="B156" s="0">
-        <v>0.021692500300573701</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C156" s="0">
-        <v>2.0880007095932349</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0">
-        <v>0.095479518072289146</v>
+        <v>0.16072385542168674</v>
       </c>
       <c r="B157" s="0">
-        <v>0.021080452107802607</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C157" s="0">
-        <v>1.9718381250950856</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0">
-        <v>0.096091566265060227</v>
+        <v>0.16175413654618473</v>
       </c>
       <c r="B158" s="0">
-        <v>0.020468403915031526</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C158" s="0">
-        <v>1.8589999358470446</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0">
-        <v>0.096703614457831308</v>
+        <v>0.16278441767068272</v>
       </c>
       <c r="B159" s="0">
-        <v>0.019856355722260445</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C159" s="0">
-        <v>1.7494861418491097</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0">
-        <v>0.097315662650602403</v>
+        <v>0.16381469879518071</v>
       </c>
       <c r="B160" s="0">
-        <v>0.01924430752948935</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C160" s="0">
-        <v>1.6432967431012786</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0">
-        <v>0.097927710843373483</v>
+        <v>0.1648449799196787</v>
       </c>
       <c r="B161" s="0">
-        <v>0.01863225933671827</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C161" s="0">
-        <v>1.5404317396035558</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0">
-        <v>0.098539759036144564</v>
+        <v>0.16587526104417671</v>
       </c>
       <c r="B162" s="0">
-        <v>0.018020211143947189</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C162" s="0">
-        <v>1.4408911313559392</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0">
-        <v>0.099151807228915645</v>
+        <v>0.1669055421686747</v>
       </c>
       <c r="B163" s="0">
-        <v>0.017451471696563161</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C163" s="0">
-        <v>1.3513739164112666</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0">
-        <v>0.09976385542168674</v>
+        <v>0.16793582329317269</v>
       </c>
       <c r="B164" s="0">
-        <v>0.016967251165243988</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C164" s="0">
-        <v>1.2774220108915422</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0">
-        <v>0.10037590361445782</v>
+        <v>0.16896610441767065</v>
       </c>
       <c r="B165" s="0">
-        <v>0.01655341779910733</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C165" s="0">
-        <v>1.215868957918449</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0">
-        <v>0.1009879518072289</v>
+        <v>0.16999638554216867</v>
       </c>
       <c r="B166" s="0">
-        <v>0.016200225587113544</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C166" s="0">
-        <v>1.1645376709988935</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0">
-        <v>0.1016</v>
+        <v>0.17102666666666666</v>
       </c>
       <c r="B167" s="0">
-        <v>0.01590074104297835</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C167" s="0">
-        <v>1.1218793319263121</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0">
-        <v>0.10221204819277108</v>
+        <v>0.17205694779116465</v>
       </c>
       <c r="B168" s="0">
-        <v>0.015649894936837237</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C168" s="0">
-        <v>1.0867615644060831</v>
+        <v>8.2698766303719147</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0">
-        <v>0.10282409638554216</v>
+        <v>0.17308722891566264</v>
       </c>
       <c r="B169" s="0">
-        <v>0.015443923767301524</v>
+        <v>0.043152994721393292</v>
       </c>
       <c r="C169" s="0">
-        <v>1.0583436687912728</v>
+        <v>8.2595357093091852</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0">
-        <v>0.10343614457831324</v>
+        <v>0.17411751004016066</v>
       </c>
       <c r="B170" s="0">
-        <v>0.015280023803178616</v>
+        <v>0.043043345190890973</v>
       </c>
       <c r="C170" s="0">
-        <v>1.0359993411217443</v>
+        <v>8.2176149291526137</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0">
-        <v>0.10404819277108433</v>
+        <v>0.17514779116465862</v>
       </c>
       <c r="B171" s="0">
-        <v>0.01515612934485408</v>
+        <v>0.042847195768302163</v>
       </c>
       <c r="C171" s="0">
-        <v>1.0192671406387019</v>
+        <v>8.142889894194985</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0">
-        <v>0.10466024096385541</v>
+        <v>0.17617807228915661</v>
       </c>
       <c r="B172" s="0">
-        <v>0.015070768161146525</v>
+        <v>0.042560333669503701</v>
       </c>
       <c r="C172" s="0">
-        <v>1.0078181969348898</v>
+        <v>8.0342215409820135</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0">
-        <v>0.10527228915662649</v>
+        <v>0.1772083534136546</v>
       </c>
       <c r="B173" s="0">
-        <v>0.015022967864357304</v>
+        <v>0.042176086250134477</v>
       </c>
       <c r="C173" s="0">
-        <v>1.0014352957965991</v>
+        <v>7.8898057026936126</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0">
-        <v>0.10588433734939758</v>
+        <v>0.17823863453815261</v>
       </c>
       <c r="B174" s="0">
-        <v>0.015012198254839038</v>
+        <v>0.04168443872684531</v>
       </c>
       <c r="C174" s="0">
-        <v>1</v>
+        <v>7.7069345563362033</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0">
-        <v>0.10649638554216867</v>
+        <v>0.1792689156626506</v>
       </c>
       <c r="B175" s="0">
-        <v>0.015038341261126088</v>
+        <v>0.041070443919198271</v>
       </c>
       <c r="C175" s="0">
-        <v>1.0034859344679434</v>
+        <v>7.4815666446492859</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0">
-        <v>0.10710843373493975</v>
+        <v>0.18029919678714859</v>
       </c>
       <c r="B176" s="0">
-        <v>0.015101684376830311</v>
+        <v>0.040311205380661248</v>
       </c>
       <c r="C176" s="0">
-        <v>1.0119573201885532</v>
+        <v>7.2075111672701251</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0">
-        <v>0.10772048192771082</v>
+        <v>0.18132947791164655</v>
       </c>
       <c r="B177" s="0">
-        <v>0.0152029367243994</v>
+        <v>0.039370492268445217</v>
       </c>
       <c r="C177" s="0">
-        <v>1.0255725625747252</v>
+        <v>6.8750434123949447</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0">
-        <v>0.10833253012048191</v>
+        <v>0.18235975903614457</v>
       </c>
       <c r="B178" s="0">
-        <v>0.01534103651552491</v>
+        <v>0.0383402111439472</v>
       </c>
       <c r="C178" s="0">
-        <v>1.0442892923364757</v>
+        <v>6.5199273322496509</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0">
-        <v>0.10894457831325299</v>
+        <v>0.18339004016064256</v>
       </c>
       <c r="B179" s="0">
-        <v>0.015487976286142617</v>
+        <v>0.037309930019449211</v>
       </c>
       <c r="C179" s="0">
-        <v>1.0643899558388998</v>
+        <v>6.1742274426241668</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0">
-        <v>0.10955662650602407</v>
+        <v>0.18442032128514055</v>
       </c>
       <c r="B180" s="0">
-        <v>0.015634916056760324</v>
+        <v>0.036279648894951222</v>
       </c>
       <c r="C180" s="0">
-        <v>1.084682230204981</v>
+        <v>5.8379437435184833</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0">
-        <v>0.11016867469879515</v>
+        <v>0.18545060240963854</v>
       </c>
       <c r="B181" s="0">
-        <v>0.015781855827378035</v>
+        <v>0.035249367770453233</v>
       </c>
       <c r="C181" s="0">
-        <v>1.1051661154347194</v>
+        <v>5.5110762349326006</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0">
-        <v>0.11078072289156625</v>
+        <v>0.18648088353413655</v>
       </c>
       <c r="B182" s="0">
-        <v>0.015928795597995746</v>
+        <v>0.034219086645955216</v>
       </c>
       <c r="C182" s="0">
-        <v>1.1258416115281151</v>
+        <v>5.1936249168665105</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0">
-        <v>0.11139277108433733</v>
+        <v>0.18751116465863454</v>
       </c>
       <c r="B183" s="0">
-        <v>0.016075735368613456</v>
+        <v>0.033188805521457233</v>
       </c>
       <c r="C183" s="0">
-        <v>1.1467087184851677</v>
+        <v>4.8855897893202309</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0">
-        <v>0.11200481927710841</v>
+        <v>0.18854144578313251</v>
       </c>
       <c r="B184" s="0">
-        <v>0.016222675139231164</v>
+        <v>0.032158524396959272</v>
       </c>
       <c r="C184" s="0">
-        <v>1.1677674363058761</v>
+        <v>4.5869708522937573</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0">
-        <v>0.11261686746987951</v>
+        <v>0.1895717269076305</v>
       </c>
       <c r="B185" s="0">
-        <v>0.016369614909848874</v>
+        <v>0.031128243272461283</v>
       </c>
       <c r="C185" s="0">
-        <v>1.1890177649902427</v>
+        <v>4.2977681057870774</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0">
-        <v>0.11322891566265059</v>
+        <v>0.19060200803212851</v>
       </c>
       <c r="B186" s="0">
-        <v>0.016516554680466585</v>
+        <v>0.030097962147963266</v>
       </c>
       <c r="C186" s="0">
-        <v>1.2104597045382664</v>
+        <v>4.0179815498001901</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0">
-        <v>0.11384096385542167</v>
+        <v>0.1916322891566265</v>
       </c>
       <c r="B187" s="0">
-        <v>0.016663494451084292</v>
+        <v>0.029067681023465276</v>
       </c>
       <c r="C187" s="0">
-        <v>1.2320932549499464</v>
+        <v>3.7476111843331097</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0">
-        <v>0.11445301204819275</v>
+        <v>0.19266257028112449</v>
       </c>
       <c r="B188" s="0">
-        <v>0.016810434221702003</v>
+        <v>0.028037399898967287</v>
       </c>
       <c r="C188" s="0">
-        <v>1.2539184162252839</v>
+        <v>3.4866570093858313</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0">
-        <v>0.11506506024096384</v>
+        <v>0.19369285140562251</v>
       </c>
       <c r="B189" s="0">
-        <v>0.016957373992319714</v>
+        <v>0.02700711877446927</v>
       </c>
       <c r="C189" s="0">
-        <v>1.2759351883642782</v>
+        <v>3.235119024958347</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0">
-        <v>0.11567710843373492</v>
+        <v>0.19472313253012047</v>
       </c>
       <c r="B190" s="0">
-        <v>0.017104313762937425</v>
+        <v>0.025976837649971309</v>
       </c>
       <c r="C190" s="0">
-        <v>1.2981435713669298</v>
+        <v>2.9929972310506758</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0">
-        <v>0.116289156626506</v>
+        <v>0.19575341365461846</v>
       </c>
       <c r="B191" s="0">
-        <v>0.017251253533555132</v>
+        <v>0.024946556525473319</v>
       </c>
       <c r="C191" s="0">
-        <v>1.3205435652332373</v>
+        <v>2.7602916276627991</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0">
-        <v>0.1169012048192771</v>
+        <v>0.19678369477911645</v>
       </c>
       <c r="B192" s="0">
-        <v>0.017398193304172842</v>
+        <v>0.02391627540097533</v>
       </c>
       <c r="C192" s="0">
-        <v>1.3431351699632028</v>
+        <v>2.5370022147947235</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0">
-        <v>0.11751325301204818</v>
+        <v>0.19781397590361446</v>
       </c>
       <c r="B193" s="0">
-        <v>0.017545133074790553</v>
+        <v>0.022885994276477313</v>
       </c>
       <c r="C193" s="0">
-        <v>1.3659183855568253</v>
+        <v>2.323128992446442</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0">
-        <v>0.11812530120481926</v>
+        <v>0.19884425702811245</v>
       </c>
       <c r="B194" s="0">
-        <v>0.01769207284540826</v>
+        <v>0.021855713151979324</v>
       </c>
       <c r="C194" s="0">
-        <v>1.3888932120141042</v>
+        <v>2.1186719606179669</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0">
-        <v>0.11873734939759034</v>
+        <v>0.19987453815261044</v>
       </c>
       <c r="B195" s="0">
-        <v>0.017839012616025971</v>
+        <v>0.020825432027481335</v>
       </c>
       <c r="C195" s="0">
-        <v>1.4120596493350408</v>
+        <v>1.923631119309293</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0">
-        <v>0.11934939759036144</v>
+        <v>0.20090481927710843</v>
       </c>
       <c r="B196" s="0">
-        <v>0.017985952386643682</v>
+        <v>0.019795150902983345</v>
       </c>
       <c r="C196" s="0">
-        <v>1.4354176975196342</v>
+        <v>1.7380064685204193</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0">
-        <v>0.11996144578313252</v>
+        <v>0.20193510040160642</v>
       </c>
       <c r="B197" s="0">
-        <v>0.018132892157261389</v>
+        <v>0.018764869778485356</v>
       </c>
       <c r="C197" s="0">
-        <v>1.4589673565678836</v>
+        <v>1.5617980082513461</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0">
-        <v>0.1205734939759036</v>
+        <v>0.20296538152610441</v>
       </c>
       <c r="B198" s="0">
-        <v>0.0182798319278791</v>
+        <v>0.017743173902211196</v>
       </c>
       <c r="C198" s="0">
-        <v>1.4827086264797911</v>
+        <v>1.3963566995708408</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0">
-        <v>0.12118554216867468</v>
+        <v>0.2039956626506024</v>
       </c>
       <c r="B199" s="0">
-        <v>0.018426771698496807</v>
+        <v>0.016900967493117456</v>
       </c>
       <c r="C199" s="0">
-        <v>1.506641507255355</v>
+        <v>1.266942449719449</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0">
-        <v>0.12179759036144577</v>
+        <v>0.20502594377510039</v>
       </c>
       <c r="B200" s="0">
-        <v>0.018573711469114521</v>
+        <v>0.016255200902237851</v>
       </c>
       <c r="C200" s="0">
-        <v>1.530765998894577</v>
+        <v>1.1719752429903643</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0">
-        <v>0.12240963855421685</v>
+        <v>0.20605622489959841</v>
       </c>
       <c r="B201" s="0">
-        <v>0.018720651239732228</v>
+        <v>0.015765327468917956</v>
       </c>
       <c r="C201" s="0">
-        <v>1.555082101397455</v>
+        <v>1.1024013770035861</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0">
-        <v>0.12302168674698793</v>
+        <v>0.2070865060240964</v>
       </c>
       <c r="B202" s="0">
-        <v>0.018867591010349939</v>
+        <v>0.015407853708921953</v>
       </c>
       <c r="C202" s="0">
-        <v>1.5795898147639904</v>
+        <v>1.052974969343464</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0">
-        <v>0.12363373493975903</v>
+        <v>0.20811678714859436</v>
       </c>
       <c r="B203" s="0">
-        <v>0.01901453078096765</v>
+        <v>0.015168574723855376</v>
       </c>
       <c r="C203" s="0">
-        <v>1.6042891389941827</v>
+        <v>1.020524194751741</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0">
-        <v>0.12424578313253011</v>
+        <v>0.20914706827309235</v>
       </c>
       <c r="B204" s="0">
-        <v>0.019161470551585357</v>
+        <v>0.015039113365624808</v>
       </c>
       <c r="C204" s="0">
-        <v>1.6291800740880311</v>
+        <v>1.0031785118716996</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0">
-        <v>0.12485783132530119</v>
+        <v>0.21017734939759036</v>
       </c>
       <c r="B205" s="0">
-        <v>0.019308410322203068</v>
+        <v>0.015015269192147789</v>
       </c>
       <c r="C205" s="0">
-        <v>1.6542626200455375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0">
-        <v>0.12546987951807229</v>
+        <v>0.21120763052208835</v>
       </c>
       <c r="B206" s="0">
-        <v>0.019455350092820779</v>
+        <v>0.015096292301306265</v>
       </c>
       <c r="C206" s="0">
-        <v>1.6795367768667009</v>
+        <v>1.0108212127802367</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0">
-        <v>0.12608192771084337</v>
+        <v>0.21223791164658634</v>
       </c>
       <c r="B207" s="0">
-        <v>0.019602289863438489</v>
+        <v>0.015284760585954545</v>
       </c>
       <c r="C207" s="0">
-        <v>1.7050025445515213</v>
+        <v>1.0362177703570472</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0">
-        <v>0.12669397590361445</v>
+        <v>0.21326819277108433</v>
       </c>
       <c r="B208" s="0">
-        <v>0.019749229634056197</v>
+        <v>0.015532058217327935</v>
       </c>
       <c r="C208" s="0">
-        <v>1.7306599230999982</v>
+        <v>1.0700197017796182</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0">
-        <v>0.12730602409638553</v>
+        <v>0.21429847389558235</v>
       </c>
       <c r="B209" s="0">
-        <v>0.019896169404673904</v>
+        <v>0.015779406831201083</v>
       </c>
       <c r="C209" s="0">
-        <v>1.756508912512132</v>
+        <v>1.1043712744293157</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0">
-        <v>0.12791807228915661</v>
+        <v>0.21532875502008031</v>
       </c>
       <c r="B210" s="0">
-        <v>0.020043109175291615</v>
+        <v>0.016026755445074224</v>
       </c>
       <c r="C210" s="0">
-        <v>1.7825495127879227</v>
+        <v>1.1392655756844024</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0">
-        <v>0.12853012048192769</v>
+        <v>0.2163590361445783</v>
       </c>
       <c r="B211" s="0">
-        <v>0.020190048945909322</v>
+        <v>0.016274104058947365</v>
       </c>
       <c r="C211" s="0">
-        <v>1.8087817239273707</v>
+        <v>1.1747026055448802</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0">
-        <v>0.1291421686746988</v>
+        <v>0.21738931726907629</v>
       </c>
       <c r="B212" s="0">
-        <v>0.020336988716527039</v>
+        <v>0.016521452672820507</v>
       </c>
       <c r="C212" s="0">
-        <v>1.8352055459304772</v>
+        <v>1.2106823640107483</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0">
-        <v>0.12975421686746988</v>
+        <v>0.2184195983935743</v>
       </c>
       <c r="B213" s="0">
-        <v>0.020483928487144747</v>
+        <v>0.016768801286693662</v>
       </c>
       <c r="C213" s="0">
-        <v>1.8618209787972391</v>
+        <v>1.2472048510820097</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0">
-        <v>0.13036626506024096</v>
+        <v>0.21944987951807229</v>
       </c>
       <c r="B214" s="0">
-        <v>0.020630868257762454</v>
+        <v>0.017016149900566803</v>
       </c>
       <c r="C214" s="0">
-        <v>1.8886280225276577</v>
+        <v>1.28427006675866</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0">
-        <v>0.13097831325301204</v>
+        <v>0.22048016064257028</v>
       </c>
       <c r="B215" s="0">
-        <v>0.020777808028380161</v>
+        <v>0.017263498514439944</v>
       </c>
       <c r="C215" s="0">
-        <v>1.9156266771217334</v>
+        <v>1.3218780110407005</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0">
-        <v>0.13159036144578312</v>
+        <v>0.22151044176706825</v>
       </c>
       <c r="B216" s="0">
-        <v>0.020924747798997875</v>
+        <v>0.017510847128313085</v>
       </c>
       <c r="C216" s="0">
-        <v>1.9428169425794675</v>
+        <v>1.3600286839281322</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0">
-        <v>0.1322024096385542</v>
+        <v>0.22254072289156626</v>
       </c>
       <c r="B217" s="0">
-        <v>0.021071687569615583</v>
+        <v>0.017758195742186234</v>
       </c>
       <c r="C217" s="0">
-        <v>1.9701988189008566</v>
+        <v>1.3987220854209552</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0">
-        <v>0.13281445783132528</v>
+        <v>0.22357100401606425</v>
       </c>
       <c r="B218" s="0">
-        <v>0.02121862734023329</v>
+        <v>0.018005544356059375</v>
       </c>
       <c r="C218" s="0">
-        <v>1.9977723060859034</v>
+        <v>1.4379582155191686</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0">
-        <v>0.13342650602409639</v>
+        <v>0.22460128514056224</v>
       </c>
       <c r="B219" s="0">
-        <v>0.021365567110851004</v>
+        <v>0.018252892969932523</v>
       </c>
       <c r="C219" s="0">
-        <v>2.0255374041346084</v>
+        <v>1.4777370742227736</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0">
-        <v>0.13403855421686747</v>
+        <v>0.22563156626506023</v>
       </c>
       <c r="B220" s="0">
-        <v>0.021512506881468711</v>
+        <v>0.018500241583805664</v>
       </c>
       <c r="C220" s="0">
-        <v>2.0534941130469693</v>
+        <v>1.5180586615317679</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0">
-        <v>0.13465060240963855</v>
+        <v>0.22666184738955825</v>
       </c>
       <c r="B221" s="0">
-        <v>0.021659446652086425</v>
+        <v>0.018747590197678819</v>
       </c>
       <c r="C221" s="0">
-        <v>2.0816424328229881</v>
+        <v>1.5589229774461557</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0">
-        <v>0.13526265060240963</v>
+        <v>0.22769212851405621</v>
       </c>
       <c r="B222" s="0">
-        <v>0.021806386422704133</v>
+        <v>0.018994938811551954</v>
       </c>
       <c r="C222" s="0">
-        <v>2.1099823634626627</v>
+        <v>1.6003300219659304</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0">
-        <v>0.13587469879518072</v>
+        <v>0.2287224096385542</v>
       </c>
       <c r="B223" s="0">
-        <v>0.02195332619332184</v>
+        <v>0.019242287425425095</v>
       </c>
       <c r="C223" s="0">
-        <v>2.1385139049659938</v>
+        <v>1.6422797950910977</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0">
-        <v>0.1364867469879518</v>
+        <v>0.22975269076305219</v>
       </c>
       <c r="B224" s="0">
-        <v>0.022100265963939547</v>
+        <v>0.019489636039298243</v>
       </c>
       <c r="C224" s="0">
-        <v>2.1672370573329824</v>
+        <v>1.6847722968216561</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0">
-        <v>0.13709879518072285</v>
+        <v>0.2307829718875502</v>
       </c>
       <c r="B225" s="0">
-        <v>0.022247205734557254</v>
+        <v>0.019736984653171391</v>
       </c>
       <c r="C225" s="0">
-        <v>2.1961518205636281</v>
+        <v>1.7278075271576059</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0">
-        <v>0.13771084337349396</v>
+        <v>0.23181325301204819</v>
       </c>
       <c r="B226" s="0">
-        <v>0.022394145505174969</v>
+        <v>0.019984333267044532</v>
       </c>
       <c r="C226" s="0">
-        <v>2.2252581946579322</v>
+        <v>1.7713854860989453</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0">
-        <v>0.13832289156626504</v>
+        <v>0.23284353413654618</v>
       </c>
       <c r="B227" s="0">
-        <v>0.022541085275792676</v>
+        <v>0.02023168188091768</v>
       </c>
       <c r="C227" s="0">
-        <v>2.2545561796158919</v>
+        <v>1.8155061736456761</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0">
-        <v>0.13893493975903612</v>
+        <v>0.23387381526104417</v>
       </c>
       <c r="B228" s="0">
-        <v>0.022688025046410383</v>
+        <v>0.020479030494790822</v>
       </c>
       <c r="C228" s="0">
-        <v>2.2840457754375083</v>
+        <v>1.8601695897977972</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0">
-        <v>0.1395469879518072</v>
+        <v>0.23490409638554216</v>
       </c>
       <c r="B229" s="0">
-        <v>0.02283496481702809</v>
+        <v>0.02072637910866397</v>
       </c>
       <c r="C229" s="0">
-        <v>2.3137269821227813</v>
+        <v>1.9053757345553095</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0">
-        <v>0.14015903614457828</v>
+        <v>0.23593437751004015</v>
       </c>
       <c r="B230" s="0">
-        <v>0.022981904587645805</v>
+        <v>0.020973727722537111</v>
       </c>
       <c r="C230" s="0">
-        <v>2.3435997996717135</v>
+        <v>1.9511246079182121</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0">
-        <v>0.14077108433734936</v>
+        <v>0.23696465863453814</v>
       </c>
       <c r="B231" s="0">
-        <v>0.023128844358263512</v>
+        <v>0.021221076336410252</v>
       </c>
       <c r="C231" s="0">
-        <v>2.373664228084301</v>
+        <v>1.9974162098865047</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0">
-        <v>0.14138313253012044</v>
+        <v>0.23799493975903613</v>
       </c>
       <c r="B232" s="0">
-        <v>0.023275784128881219</v>
+        <v>0.021468424950283401</v>
       </c>
       <c r="C232" s="0">
-        <v>2.4039202673605455</v>
+        <v>2.0442505404601903</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0">
-        <v>0.14199518072289152</v>
+        <v>0.23902522088353415</v>
       </c>
       <c r="B233" s="0">
-        <v>0.023422723899498926</v>
+        <v>0.021715773564156549</v>
       </c>
       <c r="C233" s="0">
-        <v>2.4343679175004471</v>
+        <v>2.0916275996392662</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0">
-        <v>0.14260722891566263</v>
+        <v>0.24005550200803213</v>
       </c>
       <c r="B234" s="0">
-        <v>0.02356966367011664</v>
+        <v>0.02196312217802969</v>
       </c>
       <c r="C234" s="0">
-        <v>2.4650071785040071</v>
+        <v>2.1395473874237312</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0">
-        <v>0.14321927710843371</v>
+        <v>0.2410857831325301</v>
       </c>
       <c r="B235" s="0">
-        <v>0.023716603440734355</v>
+        <v>0.022210470791902831</v>
       </c>
       <c r="C235" s="0">
-        <v>2.4958380503712241</v>
+        <v>2.1880099038135876</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0">
-        <v>0.14383132530120479</v>
+        <v>0.24211606425702809</v>
       </c>
       <c r="B236" s="0">
-        <v>0.023863543211352062</v>
+        <v>0.022457819405775972</v>
       </c>
       <c r="C236" s="0">
-        <v>2.5268605331020959</v>
+        <v>2.2370151488088341</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0">
-        <v>0.14444337349397587</v>
+        <v>0.2431463453815261</v>
       </c>
       <c r="B237" s="0">
-        <v>0.024010482981969769</v>
+        <v>0.02270516801964912</v>
       </c>
       <c r="C237" s="0">
-        <v>2.5580746266966252</v>
+        <v>2.2865631224094733</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0">
-        <v>0.14505542168674695</v>
+        <v>0.24417662650602409</v>
       </c>
       <c r="B238" s="0">
-        <v>0.024157422752587476</v>
+        <v>0.022952516633522269</v>
       </c>
       <c r="C238" s="0">
-        <v>2.589480331154812</v>
+        <v>2.3366538246155035</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0">
-        <v>0.14566746987951804</v>
+        <v>0.24520690763052208</v>
       </c>
       <c r="B239" s="0">
-        <v>0.024304362523205184</v>
+        <v>0.02319986524739541</v>
       </c>
       <c r="C239" s="0">
-        <v>2.6210776464766554</v>
+        <v>2.3872872554269224</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0">
-        <v>0.14627951807228912</v>
+        <v>0.24623718875502007</v>
       </c>
       <c r="B240" s="0">
-        <v>0.024451302293822898</v>
+        <v>0.023447213861268558</v>
       </c>
       <c r="C240" s="0">
-        <v>2.6528665726621577</v>
+        <v>2.4384634148437341</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0">
-        <v>0.14689156626506022</v>
+        <v>0.24726746987951806</v>
       </c>
       <c r="B241" s="0">
-        <v>0.024598242064440612</v>
+        <v>0.023694562475141699</v>
       </c>
       <c r="C241" s="0">
-        <v>2.6848471097113165</v>
+        <v>2.490182302865934</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0">
-        <v>0.14750361445783131</v>
+        <v>0.24829775100401605</v>
       </c>
       <c r="B242" s="0">
-        <v>0.024745181835058319</v>
+        <v>0.02394191108901484</v>
       </c>
       <c r="C242" s="0">
-        <v>2.7170192576241301</v>
+        <v>2.5424439194935262</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0">
-        <v>0.14811566265060239</v>
+        <v>0.24932803212851404</v>
       </c>
       <c r="B243" s="0">
-        <v>0.024892121605676026</v>
+        <v>0.024189259702887989</v>
       </c>
       <c r="C243" s="0">
-        <v>2.7493830164006017</v>
+        <v>2.5952482647265094</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0">
-        <v>0.14872771084337347</v>
+        <v>0.25035831325301206</v>
       </c>
       <c r="B244" s="0">
-        <v>0.025039061376293734</v>
+        <v>0.024436608316761137</v>
       </c>
       <c r="C244" s="0">
-        <v>2.7819383860407303</v>
+        <v>2.6485953385648839</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0">
-        <v>0.14933975903614455</v>
+        <v>0.25138859437751004</v>
       </c>
       <c r="B245" s="0">
-        <v>0.025186001146911448</v>
+        <v>0.024683956930634278</v>
       </c>
       <c r="C245" s="0">
-        <v>2.8146853665445173</v>
+        <v>2.7024851410086481</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0">
-        <v>0.14995180722891563</v>
+        <v>0.25241887550200803</v>
       </c>
       <c r="B246" s="0">
-        <v>0.025332940917529155</v>
+        <v>0.024931305544507426</v>
       </c>
       <c r="C246" s="0">
-        <v>2.8476239579119596</v>
+        <v>2.7569176720578037</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0">
-        <v>0.15056385542168671</v>
+        <v>0.25344915662650602</v>
       </c>
       <c r="B247" s="0">
-        <v>0.025479880688146862</v>
+        <v>0.025178654158380567</v>
       </c>
       <c r="C247" s="0">
-        <v>2.8807541601430589</v>
+        <v>2.8118929317123493</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0">
-        <v>0.15117590361445782</v>
+        <v>0.25447943775100401</v>
       </c>
       <c r="B248" s="0">
-        <v>0.025626820458764576</v>
+        <v>0.025426002772253709</v>
       </c>
       <c r="C248" s="0">
-        <v>2.9140759732378161</v>
+        <v>2.867410919972285</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0">
-        <v>0.1517879518072289</v>
+        <v>0.255509718875502</v>
       </c>
       <c r="B249" s="0">
-        <v>0.025773760229382291</v>
+        <v>0.025673351386126857</v>
       </c>
       <c r="C249" s="0">
-        <v>2.9475893971962313</v>
+        <v>2.9234716368376139</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0">
-        <v>0.15239999999999998</v>
+        <v>0.25653999999999999</v>
       </c>
       <c r="B250" s="0">
         <v>0.025920699999999998</v>
       </c>
       <c r="C250" s="0">
-        <v>2.9812944320183017</v>
+        <v>2.9800750823083311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new venturi sizing code, fixed missing Maelstrom files
</commit_message>
<xml_diff>
--- a/REGEN/Contour_Maelstrom.xlsx
+++ b/REGEN/Contour_Maelstrom.xlsx
@@ -59,7 +59,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="true"/>
+    <col min="1" max="1" width="14.5546875" customWidth="true"/>
     <col min="2" max="2" width="13.5546875" customWidth="true"/>
     <col min="3" max="3" width="11.5546875" customWidth="true"/>
   </cols>
@@ -72,2746 +72,2746 @@
         <v>0.043179999999999996</v>
       </c>
       <c r="C1" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.0008772690763052209</v>
+        <v>0.00095887550200803213</v>
       </c>
       <c r="B2" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C2" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.0017545381526104418</v>
+        <v>0.0019177510040160643</v>
       </c>
       <c r="B3" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C3" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.0026318072289156628</v>
+        <v>0.0028766265060240965</v>
       </c>
       <c r="B4" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C4" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.0035090763052208836</v>
+        <v>0.0038355020080321285</v>
       </c>
       <c r="B5" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C5" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.0043863453815261048</v>
+        <v>0.0047943775100401601</v>
       </c>
       <c r="B6" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C6" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.0052636144578313256</v>
+        <v>0.005753253012048193</v>
       </c>
       <c r="B7" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C7" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.0061408835341365464</v>
+        <v>0.0067121285140562242</v>
       </c>
       <c r="B8" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C8" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.0070181526104417672</v>
+        <v>0.0076710040160642571</v>
       </c>
       <c r="B9" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C9" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.0078954216867469871</v>
+        <v>0.0086298795180722882</v>
       </c>
       <c r="B10" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C10" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.0087726907630522096</v>
+        <v>0.0095887550200803202</v>
       </c>
       <c r="B11" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C11" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.0096499598393574287</v>
+        <v>0.010547630522088354</v>
       </c>
       <c r="B12" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C12" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.010527228915662651</v>
+        <v>0.011506506024096386</v>
       </c>
       <c r="B13" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C13" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.01140449799196787</v>
+        <v>0.012465381526104418</v>
       </c>
       <c r="B14" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C14" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.012281767068273093</v>
+        <v>0.013424257028112448</v>
       </c>
       <c r="B15" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C15" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.013159036144578312</v>
+        <v>0.014383132530120482</v>
       </c>
       <c r="B16" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C16" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.014036305220883534</v>
+        <v>0.015342008032128514</v>
       </c>
       <c r="B17" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C17" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.014913574297188755</v>
+        <v>0.016300883534136546</v>
       </c>
       <c r="B18" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C18" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.015790843373493974</v>
+        <v>0.017259759036144576</v>
       </c>
       <c r="B19" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C19" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.016668112449799197</v>
+        <v>0.01821863453815261</v>
       </c>
       <c r="B20" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C20" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.017545381526104419</v>
+        <v>0.01917751004016064</v>
       </c>
       <c r="B21" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C21" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.018422650602409638</v>
+        <v>0.020136385542168674</v>
       </c>
       <c r="B22" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C22" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.019299919678714857</v>
+        <v>0.021095261044176708</v>
       </c>
       <c r="B23" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C23" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.02017718875502008</v>
+        <v>0.022054136546184738</v>
       </c>
       <c r="B24" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C24" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.021054457831325302</v>
+        <v>0.023013012048192772</v>
       </c>
       <c r="B25" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C25" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.021931726907630525</v>
+        <v>0.023971887550200806</v>
       </c>
       <c r="B26" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C26" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.022808995983935741</v>
+        <v>0.024930763052208836</v>
       </c>
       <c r="B27" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C27" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.023686265060240963</v>
+        <v>0.025889638554216866</v>
       </c>
       <c r="B28" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C28" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.024563534136546186</v>
+        <v>0.026848514056224897</v>
       </c>
       <c r="B29" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C29" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.025440803212851405</v>
+        <v>0.027807389558232931</v>
       </c>
       <c r="B30" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C30" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.026318072289156624</v>
+        <v>0.028766265060240964</v>
       </c>
       <c r="B31" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C31" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.027195341365461846</v>
+        <v>0.029725140562248994</v>
       </c>
       <c r="B32" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C32" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.028072610441767069</v>
+        <v>0.030684016064257028</v>
       </c>
       <c r="B33" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C33" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.028949879518072288</v>
+        <v>0.031642891566265062</v>
       </c>
       <c r="B34" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C34" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.02982714859437751</v>
+        <v>0.032601767068273092</v>
       </c>
       <c r="B35" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C35" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.030704417670682729</v>
+        <v>0.033560642570281123</v>
       </c>
       <c r="B36" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C36" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.031581686746987948</v>
+        <v>0.034519518072289153</v>
       </c>
       <c r="B37" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C37" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.032458955823293167</v>
+        <v>0.03547839357429719</v>
       </c>
       <c r="B38" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C38" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.033336224899598394</v>
+        <v>0.03643726907630522</v>
       </c>
       <c r="B39" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C39" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.034213493975903612</v>
+        <v>0.037396144578313258</v>
       </c>
       <c r="B40" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C40" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.035090763052208838</v>
+        <v>0.038355020080321281</v>
       </c>
       <c r="B41" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C41" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.035968032128514058</v>
+        <v>0.039313895582329318</v>
       </c>
       <c r="B42" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C42" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.036845301204819277</v>
+        <v>0.040272771084337349</v>
       </c>
       <c r="B43" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C43" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.037722570281124496</v>
+        <v>0.041231646586345379</v>
       </c>
       <c r="B44" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C44" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.038599839357429715</v>
+        <v>0.042190522088353416</v>
       </c>
       <c r="B45" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C45" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.039477108433734941</v>
+        <v>0.043149397590361446</v>
       </c>
       <c r="B46" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C46" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.04035437751004016</v>
+        <v>0.044108273092369477</v>
       </c>
       <c r="B47" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C47" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.041231646586345379</v>
+        <v>0.045067148594377507</v>
       </c>
       <c r="B48" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C48" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.042108915662650605</v>
+        <v>0.046026024096385544</v>
       </c>
       <c r="B49" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C49" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.042986184738955824</v>
+        <v>0.046984899598393574</v>
       </c>
       <c r="B50" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C50" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.04386345381526105</v>
+        <v>0.047943775100401612</v>
       </c>
       <c r="B51" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C51" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.044740722891566262</v>
+        <v>0.048902650602409635</v>
       </c>
       <c r="B52" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C52" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.045617991967871481</v>
+        <v>0.049861526104417672</v>
       </c>
       <c r="B53" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.046495261044176707</v>
+        <v>0.050820401606425702</v>
       </c>
       <c r="B54" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C54" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.047372530120481926</v>
+        <v>0.051779277108433733</v>
       </c>
       <c r="B55" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.048249799196787145</v>
+        <v>0.05273815261044177</v>
       </c>
       <c r="B56" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C56" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.049127068273092371</v>
+        <v>0.053697028112449793</v>
       </c>
       <c r="B57" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C57" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.05000433734939759</v>
+        <v>0.054655903614457831</v>
       </c>
       <c r="B58" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C58" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.050881606425702809</v>
+        <v>0.055614779116465861</v>
       </c>
       <c r="B59" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.051758875502008028</v>
+        <v>0.056573654618473898</v>
       </c>
       <c r="B60" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C60" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.052636144578313247</v>
+        <v>0.057532530120481928</v>
       </c>
       <c r="B61" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C61" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0.053513413654618473</v>
+        <v>0.058491405622489966</v>
       </c>
       <c r="B62" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C62" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.054390682730923692</v>
+        <v>0.059450281124497989</v>
       </c>
       <c r="B63" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C63" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.055267951807228918</v>
+        <v>0.060409156626506026</v>
       </c>
       <c r="B64" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C64" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0.056145220883534137</v>
+        <v>0.061368032128514057</v>
       </c>
       <c r="B65" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C65" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.057022489959839356</v>
+        <v>0.062326907630522087</v>
       </c>
       <c r="B66" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C66" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.057899759036144576</v>
+        <v>0.063285783132530124</v>
       </c>
       <c r="B67" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C67" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0.058777028112449795</v>
+        <v>0.064244658634538154</v>
       </c>
       <c r="B68" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C68" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.059654297188755021</v>
+        <v>0.065203534136546185</v>
       </c>
       <c r="B69" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C69" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.06053156626506024</v>
+        <v>0.066162409638554229</v>
       </c>
       <c r="B70" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C70" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0.061408835341365459</v>
+        <v>0.067121285140562245</v>
       </c>
       <c r="B71" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C71" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.062286104417670685</v>
+        <v>0.068080160642570276</v>
       </c>
       <c r="B72" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C72" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.063163373493975897</v>
+        <v>0.069039036144578306</v>
       </c>
       <c r="B73" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C73" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0.064040642570281123</v>
+        <v>0.06999791164658635</v>
       </c>
       <c r="B74" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C74" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.064917911646586335</v>
+        <v>0.07095678714859438</v>
       </c>
       <c r="B75" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C75" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.065795180722891561</v>
+        <v>0.07191566265060241</v>
       </c>
       <c r="B76" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C76" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0.066672449799196787</v>
+        <v>0.072874538152610441</v>
       </c>
       <c r="B77" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C77" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.067549718875502013</v>
+        <v>0.073833413654618471</v>
       </c>
       <c r="B78" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C78" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.068426987951807225</v>
+        <v>0.074792289156626515</v>
       </c>
       <c r="B79" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C79" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0.069304257028112451</v>
+        <v>0.075751164658634546</v>
       </c>
       <c r="B80" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C80" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.070181526104417677</v>
+        <v>0.076710040160642562</v>
       </c>
       <c r="B81" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C81" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.071058795180722889</v>
+        <v>0.077668915662650592</v>
       </c>
       <c r="B82" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C82" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.071936064257028115</v>
+        <v>0.078627791164658636</v>
       </c>
       <c r="B83" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C83" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.072813333333333341</v>
+        <v>0.079586666666666667</v>
       </c>
       <c r="B84" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C84" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.073690602409638553</v>
+        <v>0.080545542168674697</v>
       </c>
       <c r="B85" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C85" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.074567871485943765</v>
+        <v>0.081504417670682727</v>
       </c>
       <c r="B86" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C86" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.075445140562248991</v>
+        <v>0.082463293172690758</v>
       </c>
       <c r="B87" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C87" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.076322409638554203</v>
+        <v>0.083422168674698802</v>
       </c>
       <c r="B88" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C88" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.077199678714859429</v>
+        <v>0.084381044176706832</v>
       </c>
       <c r="B89" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C89" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.078076947791164655</v>
+        <v>0.085339919678714862</v>
       </c>
       <c r="B90" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C90" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.078954216867469881</v>
+        <v>0.086298795180722893</v>
       </c>
       <c r="B91" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C91" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>0.079831485943775093</v>
+        <v>0.087257670682730923</v>
       </c>
       <c r="B92" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C92" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>0.08070875502008032</v>
+        <v>0.088216546184738953</v>
       </c>
       <c r="B93" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C93" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.081586024096385546</v>
+        <v>0.089175421686746983</v>
       </c>
       <c r="B94" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C94" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>0.082463293172690758</v>
+        <v>0.090134297188755014</v>
       </c>
       <c r="B95" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C95" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>0.083340562248995984</v>
+        <v>0.091093172690763058</v>
       </c>
       <c r="B96" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C96" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.08421783132530121</v>
+        <v>0.092052048192771088</v>
       </c>
       <c r="B97" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C97" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>0.085095100401606422</v>
+        <v>0.093010923694779119</v>
       </c>
       <c r="B98" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C98" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>0.085972369477911648</v>
+        <v>0.093969799196787149</v>
       </c>
       <c r="B99" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C99" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.086849638554216874</v>
+        <v>0.094928674698795179</v>
       </c>
       <c r="B100" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C100" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>0.0877269076305221</v>
+        <v>0.095887550200803223</v>
       </c>
       <c r="B101" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C101" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>0.088604176706827298</v>
+        <v>0.096846425702811254</v>
       </c>
       <c r="B102" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C102" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.089481445783132524</v>
+        <v>0.09780530120481927</v>
       </c>
       <c r="B103" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C103" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0">
-        <v>0.09035871485943775</v>
+        <v>0.0987641767068273</v>
       </c>
       <c r="B104" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C104" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.091235983935742962</v>
+        <v>0.099723052208835344</v>
       </c>
       <c r="B105" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C105" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.092113253012048188</v>
+        <v>0.10068192771084337</v>
       </c>
       <c r="B106" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C106" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>0.092990522088353414</v>
+        <v>0.1016408032128514</v>
       </c>
       <c r="B107" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C107" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.093867791164658626</v>
+        <v>0.10259967871485944</v>
       </c>
       <c r="B108" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C108" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.094745060240963852</v>
+        <v>0.10355855421686747</v>
       </c>
       <c r="B109" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C109" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>0.095622329317269078</v>
+        <v>0.10451742971887551</v>
       </c>
       <c r="B110" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C110" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.09649959839357429</v>
+        <v>0.10547630522088354</v>
       </c>
       <c r="B111" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C111" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.097376867469879516</v>
+        <v>0.10643518072289157</v>
       </c>
       <c r="B112" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C112" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>0.098254136546184742</v>
+        <v>0.10739405622489959</v>
       </c>
       <c r="B113" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C113" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.099131405622489968</v>
+        <v>0.10835293172690763</v>
       </c>
       <c r="B114" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C114" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.10000867469879518</v>
+        <v>0.10931180722891566</v>
       </c>
       <c r="B115" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C115" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>0.10088594377510041</v>
+        <v>0.11027068273092369</v>
       </c>
       <c r="B116" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C116" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.10176321285140562</v>
+        <v>0.11122955823293172</v>
       </c>
       <c r="B117" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C117" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.10264048192771083</v>
+        <v>0.11218843373493977</v>
       </c>
       <c r="B118" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C118" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>0.10351775100401606</v>
+        <v>0.1131473092369478</v>
       </c>
       <c r="B119" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C119" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.10439502008032128</v>
+        <v>0.11410618473895583</v>
       </c>
       <c r="B120" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C120" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.10527228915662649</v>
+        <v>0.11506506024096386</v>
       </c>
       <c r="B121" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C121" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0">
-        <v>0.10614955823293172</v>
+        <v>0.11602393574297189</v>
       </c>
       <c r="B122" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C122" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>0.10702682730923695</v>
+        <v>0.11698281124497993</v>
       </c>
       <c r="B123" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C123" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.10790409638554217</v>
+        <v>0.11794168674698795</v>
       </c>
       <c r="B124" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C124" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0">
-        <v>0.10878136546184738</v>
+        <v>0.11890056224899598</v>
       </c>
       <c r="B125" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C125" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>0.10965863453815261</v>
+        <v>0.11985943775100401</v>
       </c>
       <c r="B126" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C126" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.11053590361445784</v>
+        <v>0.12081831325301205</v>
       </c>
       <c r="B127" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C127" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0">
-        <v>0.11141317269076305</v>
+        <v>0.12177718875502008</v>
       </c>
       <c r="B128" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C128" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>0.11229044176706827</v>
+        <v>0.12273606425702811</v>
       </c>
       <c r="B129" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C129" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.1131677108433735</v>
+        <v>0.12369493975903614</v>
       </c>
       <c r="B130" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C130" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0">
-        <v>0.11404497991967871</v>
+        <v>0.12465381526104417</v>
       </c>
       <c r="B131" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C131" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.11492224899598394</v>
+        <v>0.1256126907630522</v>
       </c>
       <c r="B132" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C132" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.11579951807228915</v>
+        <v>0.12657156626506025</v>
       </c>
       <c r="B133" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C133" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0">
-        <v>0.11667678714859436</v>
+        <v>0.12753044176706827</v>
       </c>
       <c r="B134" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C134" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.11755405622489959</v>
+        <v>0.12848931726907631</v>
       </c>
       <c r="B135" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C135" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.11843132530120482</v>
+        <v>0.12944819277108432</v>
       </c>
       <c r="B136" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C136" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0">
-        <v>0.11930859437751004</v>
+        <v>0.13040706827309237</v>
       </c>
       <c r="B137" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C137" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.12018586345381525</v>
+        <v>0.13136594377510041</v>
       </c>
       <c r="B138" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C138" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.12106313253012048</v>
+        <v>0.13232481927710846</v>
       </c>
       <c r="B139" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C139" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0">
-        <v>0.12194040160642571</v>
+        <v>0.13328369477911647</v>
       </c>
       <c r="B140" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C140" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.12281767068273092</v>
+        <v>0.13424257028112449</v>
       </c>
       <c r="B141" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C141" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.12369493975903614</v>
+        <v>0.13520144578313253</v>
       </c>
       <c r="B142" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C142" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0">
-        <v>0.12457220883534137</v>
+        <v>0.13616032128514055</v>
       </c>
       <c r="B143" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C143" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.12544947791164657</v>
+        <v>0.1371191967871486</v>
       </c>
       <c r="B144" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C144" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.12632674698795179</v>
+        <v>0.13807807228915661</v>
       </c>
       <c r="B145" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C145" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0">
-        <v>0.12720401606425702</v>
+        <v>0.13903694779116466</v>
       </c>
       <c r="B146" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C146" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>0.12808128514056225</v>
+        <v>0.1399958232931727</v>
       </c>
       <c r="B147" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C147" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.12895855421686747</v>
+        <v>0.14095469879518074</v>
       </c>
       <c r="B148" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C148" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0">
-        <v>0.12983582329317267</v>
+        <v>0.14191357429718876</v>
       </c>
       <c r="B149" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C149" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>0.1307130923694779</v>
+        <v>0.14287244979919678</v>
       </c>
       <c r="B150" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C150" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.13159036144578312</v>
+        <v>0.14383132530120482</v>
       </c>
       <c r="B151" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C151" s="0">
-        <v>7.3480451087897176</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0">
-        <v>0.13246763052208835</v>
+        <v>0.14479020080321284</v>
       </c>
       <c r="B152" s="0">
-        <v>0.043179177500336327</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C152" s="0">
-        <v>7.3477651779388937</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>0.13334489959839357</v>
+        <v>0.14574907630522088</v>
       </c>
       <c r="B153" s="0">
-        <v>0.043138827483513054</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C153" s="0">
-        <v>7.3340389359190654</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0">
-        <v>0.1342221686746988</v>
+        <v>0.1467079518072289</v>
       </c>
       <c r="B154" s="0">
-        <v>0.043037209692649056</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C154" s="0">
-        <v>7.2995275177448633</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0">
-        <v>0.13509943775100403</v>
+        <v>0.14766682730923694</v>
       </c>
       <c r="B155" s="0">
-        <v>0.042872817081216472</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C155" s="0">
-        <v>7.2438688654090022</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0">
-        <v>0.13597670682730922</v>
+        <v>0.14862570281124499</v>
       </c>
       <c r="B156" s="0">
-        <v>0.04264310458260305</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C156" s="0">
-        <v>7.1664515434123128</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0">
-        <v>0.13685397590361445</v>
+        <v>0.14958457831325303</v>
       </c>
       <c r="B157" s="0">
-        <v>0.042344278692853808</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C157" s="0">
-        <v>7.0663641874026189</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0">
-        <v>0.13773124497991968</v>
+        <v>0.15054345381526105</v>
       </c>
       <c r="B158" s="0">
-        <v>0.041970948727219508</v>
+        <v>0.043179999999999996</v>
       </c>
       <c r="C158" s="0">
-        <v>6.9423117208563223</v>
+        <v>6.6128135255224567</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0">
-        <v>0.1386085140562249</v>
+        <v>0.15150232931726909</v>
       </c>
       <c r="B159" s="0">
-        <v>0.041515555914270363</v>
+        <v>0.043166394565478709</v>
       </c>
       <c r="C159" s="0">
-        <v>6.7924781986975518</v>
+        <v>6.6086469656694868</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0">
-        <v>0.13948578313253013</v>
+        <v>0.15246120481927711</v>
       </c>
       <c r="B160" s="0">
-        <v>0.040967415504208113</v>
+        <v>0.043085478963667503</v>
       </c>
       <c r="C160" s="0">
-        <v>6.614296680126035</v>
+        <v>6.58389430967362</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0">
-        <v>0.14036305220883535</v>
+        <v>0.15342008032128512</v>
       </c>
       <c r="B161" s="0">
-        <v>0.040311025964482994</v>
+        <v>0.042930409964303105</v>
       </c>
       <c r="C161" s="0">
-        <v>6.4040430239947961</v>
+        <v>6.5365873904226328</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0">
-        <v>0.14124032128514055</v>
+        <v>0.15437895582329317</v>
       </c>
       <c r="B162" s="0">
-        <v>0.039522845625481542</v>
+        <v>0.042698364546790608</v>
       </c>
       <c r="C162" s="0">
-        <v>6.1560614991563316</v>
+        <v>6.466115856432249</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0">
-        <v>0.14211759036144578</v>
+        <v>0.15533783132530118</v>
       </c>
       <c r="B163" s="0">
-        <v>0.038646015850478291</v>
+        <v>0.04238484236185508</v>
       </c>
       <c r="C163" s="0">
-        <v>5.8859422006254709</v>
+        <v>6.3715067091828424</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0">
-        <v>0.14299485943775101</v>
+        <v>0.15629670682730923</v>
       </c>
       <c r="B164" s="0">
-        <v>0.037768746774173065</v>
+        <v>0.041983183327508354</v>
       </c>
       <c r="C164" s="0">
-        <v>5.6217520473418068</v>
+        <v>6.2513200049013458</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0">
-        <v>0.14387212851405623</v>
+        <v>0.15725558232931727</v>
       </c>
       <c r="B165" s="0">
-        <v>0.036891477697867839</v>
+        <v>0.041483740146659717</v>
       </c>
       <c r="C165" s="0">
-        <v>5.3636278908310029</v>
+        <v>6.1034699486384767</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0">
-        <v>0.14474939759036146</v>
+        <v>0.15821445783132532</v>
       </c>
       <c r="B166" s="0">
-        <v>0.036014208621562613</v>
+        <v>0.040872424322912</v>
       </c>
       <c r="C166" s="0">
-        <v>5.1115697310930637</v>
+        <v>5.9249105354508975</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0">
-        <v>0.14562666666666668</v>
+        <v>0.15917333333333333</v>
       </c>
       <c r="B167" s="0">
-        <v>0.035136939545257387</v>
+        <v>0.04012799382996244</v>
       </c>
       <c r="C167" s="0">
-        <v>4.8655775681279847</v>
+        <v>5.7110491306598821</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0">
-        <v>0.14650393574297191</v>
+        <v>0.16013220883534138</v>
       </c>
       <c r="B168" s="0">
-        <v>0.034259670468952168</v>
+        <v>0.039222931329655403</v>
       </c>
       <c r="C168" s="0">
-        <v>4.6256514019357731</v>
+        <v>5.4563358638756201</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0">
-        <v>0.14738120481927711</v>
+        <v>0.16109108433734939</v>
       </c>
       <c r="B169" s="0">
-        <v>0.03338240139264697</v>
+        <v>0.038264055827647386</v>
       </c>
       <c r="C169" s="0">
-        <v>4.391791232516427</v>
+        <v>5.1928168246791691</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0">
-        <v>0.14825847389558233</v>
+        <v>0.16204995983935744</v>
       </c>
       <c r="B170" s="0">
-        <v>0.032505132316341744</v>
+        <v>0.037305180325639342</v>
       </c>
       <c r="C170" s="0">
-        <v>4.1639970598699376</v>
+        <v>4.9358197051047812</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0">
-        <v>0.14913574297188753</v>
+        <v>0.16300883534136545</v>
       </c>
       <c r="B171" s="0">
-        <v>0.031627863240036545</v>
+        <v>0.036346304823631326</v>
       </c>
       <c r="C171" s="0">
-        <v>3.9422688839963169</v>
+        <v>4.6853445051524716</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0">
-        <v>0.15001301204819276</v>
+        <v>0.16396771084337347</v>
       </c>
       <c r="B172" s="0">
-        <v>0.030750594163731319</v>
+        <v>0.035387429321623309</v>
       </c>
       <c r="C172" s="0">
-        <v>3.7266067048955516</v>
+        <v>4.4413912248222323</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0">
-        <v>0.15089028112449798</v>
+        <v>0.16492658634538152</v>
       </c>
       <c r="B173" s="0">
-        <v>0.029873325087426093</v>
+        <v>0.034428553819615265</v>
       </c>
       <c r="C173" s="0">
-        <v>3.5170105225676491</v>
+        <v>4.2039598641140579</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0">
-        <v>0.15176755020080321</v>
+        <v>0.16588546184738956</v>
       </c>
       <c r="B174" s="0">
-        <v>0.028996056011120867</v>
+        <v>0.033469678317607221</v>
       </c>
       <c r="C174" s="0">
-        <v>3.3134803370126091</v>
+        <v>3.9730504230279524</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0">
-        <v>0.15264481927710841</v>
+        <v>0.1668443373493976</v>
       </c>
       <c r="B175" s="0">
-        <v>0.028118786934815669</v>
+        <v>0.032510802815599177</v>
       </c>
       <c r="C175" s="0">
-        <v>3.1160161482304378</v>
+        <v>3.7486629015639181</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0">
-        <v>0.15352208835341363</v>
+        <v>0.16780321285140562</v>
       </c>
       <c r="B176" s="0">
-        <v>0.027241517858510443</v>
+        <v>0.031551927313591161</v>
       </c>
       <c r="C176" s="0">
-        <v>2.9246179562211232</v>
+        <v>3.5307972997219621</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0">
-        <v>0.15439935742971886</v>
+        <v>0.16876208835341366</v>
       </c>
       <c r="B177" s="0">
-        <v>0.026364248782205217</v>
+        <v>0.030593051811583116</v>
       </c>
       <c r="C177" s="0">
-        <v>2.7392857609846706</v>
+        <v>3.3194536175020688</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0">
-        <v>0.15527662650602409</v>
+        <v>0.16972096385542168</v>
       </c>
       <c r="B178" s="0">
-        <v>0.025486979705899991</v>
+        <v>0.0296341763095751</v>
       </c>
       <c r="C178" s="0">
-        <v>2.5600195625210809</v>
+        <v>3.1146318549042533</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0">
-        <v>0.15615389558232931</v>
+        <v>0.17067983935742973</v>
       </c>
       <c r="B179" s="0">
-        <v>0.024609710629594765</v>
+        <v>0.028675300807567056</v>
       </c>
       <c r="C179" s="0">
-        <v>2.3868193608303532</v>
+        <v>2.9163320119285023</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0">
-        <v>0.15703116465863454</v>
+        <v>0.17163871485943774</v>
       </c>
       <c r="B180" s="0">
-        <v>0.023732441553289539</v>
+        <v>0.027716425305559039</v>
       </c>
       <c r="C180" s="0">
-        <v>2.2196851559124884</v>
+        <v>2.7245540885748278</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0">
-        <v>0.15790843373493976</v>
+        <v>0.17259759036144579</v>
       </c>
       <c r="B181" s="0">
-        <v>0.022855172476984313</v>
+        <v>0.026757549803550995</v>
       </c>
       <c r="C181" s="0">
-        <v>2.0586169477674861</v>
+        <v>2.5392980848432183</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0">
-        <v>0.15878570281124496</v>
+        <v>0.17355646586345383</v>
       </c>
       <c r="B182" s="0">
-        <v>0.021977903400679115</v>
+        <v>0.025798674301542951</v>
       </c>
       <c r="C182" s="0">
-        <v>1.9036147363953513</v>
+        <v>2.3605640007336794</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0">
-        <v>0.15966297188755019</v>
+        <v>0.17451534136546185</v>
       </c>
       <c r="B183" s="0">
-        <v>0.021100634324373889</v>
+        <v>0.024839798799534935</v>
       </c>
       <c r="C183" s="0">
-        <v>1.7546785217960745</v>
+        <v>2.1883518362462171</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0">
-        <v>0.16054024096385541</v>
+        <v>0.17547421686746989</v>
       </c>
       <c r="B184" s="0">
-        <v>0.020223365248068663</v>
+        <v>0.02388092329752689</v>
       </c>
       <c r="C184" s="0">
-        <v>1.6118083039696598</v>
+        <v>2.0226615913808192</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0">
-        <v>0.16141751004016064</v>
+        <v>0.17643309236947791</v>
       </c>
       <c r="B185" s="0">
-        <v>0.019346096171763437</v>
+        <v>0.022922047795518874</v>
       </c>
       <c r="C185" s="0">
-        <v>1.4750040829161075</v>
+        <v>1.8634932661374972</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0">
-        <v>0.16229477911646586</v>
+        <v>0.17739196787148595</v>
       </c>
       <c r="B186" s="0">
-        <v>0.018493455175667396</v>
+        <v>0.02196317229351083</v>
       </c>
       <c r="C186" s="0">
-        <v>1.3478533914019819</v>
+        <v>1.7108468605162417</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0">
-        <v>0.16317204819277109</v>
+        <v>0.17835084337349397</v>
       </c>
       <c r="B187" s="0">
-        <v>0.017796062217276289</v>
+        <v>0.021004296791502813</v>
       </c>
       <c r="C187" s="0">
-        <v>1.2481143273854132</v>
+        <v>1.5647223745170609</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0">
-        <v>0.16404931726907632</v>
+        <v>0.17930971887550201</v>
       </c>
       <c r="B188" s="0">
-        <v>0.017239523776832362</v>
+        <v>0.020045421289494769</v>
       </c>
       <c r="C188" s="0">
-        <v>1.1712701280009714</v>
+        <v>1.4251198081399468</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0">
-        <v>0.16492658634538152</v>
+        <v>0.18026859437751003</v>
       </c>
       <c r="B189" s="0">
-        <v>0.016798483301277912</v>
+        <v>0.019145340378242136</v>
       </c>
       <c r="C189" s="0">
-        <v>1.1121072748644763</v>
+        <v>1.3000114698923837</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0">
-        <v>0.16580385542168674</v>
+        <v>0.18122746987951807</v>
       </c>
       <c r="B190" s="0">
-        <v>0.016457056684091087</v>
+        <v>0.018437059540459856</v>
       </c>
       <c r="C190" s="0">
-        <v>1.0673598634509929</v>
+        <v>1.2056029906054122</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0">
-        <v>0.16668112449799197</v>
+        <v>0.18218634538152612</v>
       </c>
       <c r="B191" s="0">
-        <v>0.016204912278723324</v>
+        <v>0.01788421113480837</v>
       </c>
       <c r="C191" s="0">
-        <v>1.0349036212264258</v>
+        <v>1.1343852657709359</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0">
-        <v>0.16755839357429719</v>
+        <v>0.18314522088353416</v>
       </c>
       <c r="B192" s="0">
-        <v>0.01603532814974297</v>
+        <v>0.017459591057383601</v>
       </c>
       <c r="C192" s="0">
-        <v>1.0133564623106308</v>
+        <v>1.0811579220710357</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0">
-        <v>0.16843566265060242</v>
+        <v>0.18410409638554218</v>
       </c>
       <c r="B193" s="0">
-        <v>0.015944161838408015</v>
+        <v>0.017146522161506472</v>
       </c>
       <c r="C193" s="0">
-        <v>1.0018666627031871</v>
+        <v>1.0427329335771689</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0">
-        <v>0.16931293172690765</v>
+        <v>0.18506297188755019</v>
       </c>
       <c r="B194" s="0">
-        <v>0.015929301453550742</v>
+        <v>0.016934537564160419</v>
       </c>
       <c r="C194" s="0">
-        <v>1</v>
+        <v>1.0171094367669416</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0">
-        <v>0.17019020080321284</v>
+        <v>0.18602184738955824</v>
       </c>
       <c r="B195" s="0">
-        <v>0.015990410023237825</v>
+        <v>0.016817290602423818</v>
       </c>
       <c r="C195" s="0">
-        <v>1.0076871899665227</v>
+        <v>1.0030741949672455</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0">
-        <v>0.17106746987951807</v>
+        <v>0.18698072289156625</v>
       </c>
       <c r="B196" s="0">
-        <v>0.01612888618208877</v>
+        <v>0.016791500235609228</v>
       </c>
       <c r="C196" s="0">
-        <v>1.0252158035231778</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0">
-        <v>0.1719447389558233</v>
+        <v>0.1879395983935743</v>
       </c>
       <c r="B197" s="0">
-        <v>0.016332975425408</v>
+        <v>0.016856465345219639</v>
       </c>
       <c r="C197" s="0">
-        <v>1.0513253949065233</v>
+        <v>1.0077528251044863</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0">
-        <v>0.17282200803212852</v>
+        <v>0.18889847389558231</v>
       </c>
       <c r="B198" s="0">
-        <v>0.016543589096626718</v>
+        <v>0.017013966048167781</v>
       </c>
       <c r="C198" s="0">
-        <v>1.0786138861908896</v>
+        <v>1.0266729598387934</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0">
-        <v>0.17369927710843375</v>
+        <v>0.18985734939759036</v>
       </c>
       <c r="B199" s="0">
-        <v>0.016754202767845436</v>
+        <v>0.017240912327645009</v>
       </c>
       <c r="C199" s="0">
-        <v>1.1062520082481162</v>
+        <v>1.0542448473181347</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0">
-        <v>0.17457654618473897</v>
+        <v>0.1908162248995984</v>
       </c>
       <c r="B200" s="0">
-        <v>0.016964816439064154</v>
+        <v>0.01747111796827942</v>
       </c>
       <c r="C200" s="0">
-        <v>1.1342397610782034</v>
+        <v>1.0825859652439427</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0">
-        <v>0.1754538152610442</v>
+        <v>0.19177510040160645</v>
       </c>
       <c r="B201" s="0">
-        <v>0.017175430110282872</v>
+        <v>0.017701323608913837</v>
       </c>
       <c r="C201" s="0">
-        <v>1.1625771446811515</v>
+        <v>1.1113029923374258</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0">
-        <v>0.17633108433734937</v>
+        <v>0.19273397590361446</v>
       </c>
       <c r="B202" s="0">
-        <v>0.017386043781501576</v>
+        <v>0.017931529249548241</v>
       </c>
       <c r="C202" s="0">
-        <v>1.1912641590569579</v>
+        <v>1.140395928598581</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0">
-        <v>0.1772083534136546</v>
+        <v>0.19369285140562251</v>
       </c>
       <c r="B203" s="0">
-        <v>0.017596657452720294</v>
+        <v>0.018161734890182659</v>
       </c>
       <c r="C203" s="0">
-        <v>1.2203008042056269</v>
+        <v>1.1698647740274113</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0">
-        <v>0.17808562248995982</v>
+        <v>0.19465172690763052</v>
       </c>
       <c r="B204" s="0">
-        <v>0.017807271123939011</v>
+        <v>0.018391940530817063</v>
       </c>
       <c r="C204" s="0">
-        <v>1.2496870801271571</v>
+        <v>1.1997095286239143</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0">
-        <v>0.17896289156626505</v>
+        <v>0.19561060240963854</v>
       </c>
       <c r="B205" s="0">
-        <v>0.018017884795157729</v>
+        <v>0.018622146171451474</v>
       </c>
       <c r="C205" s="0">
-        <v>1.2794229868215472</v>
+        <v>1.2299301923880921</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0">
-        <v>0.17984016064257027</v>
+        <v>0.19656947791164659</v>
       </c>
       <c r="B206" s="0">
-        <v>0.018228498466376447</v>
+        <v>0.018852351812085891</v>
       </c>
       <c r="C206" s="0">
-        <v>1.3095085242887981</v>
+        <v>1.2605267653199448</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0">
-        <v>0.1807174297188755</v>
+        <v>0.1975283534136546</v>
       </c>
       <c r="B207" s="0">
-        <v>0.018439112137595165</v>
+        <v>0.019082557452720295</v>
       </c>
       <c r="C207" s="0">
-        <v>1.3399436925289099</v>
+        <v>1.2914992474194693</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0">
-        <v>0.1815946987951807</v>
+        <v>0.19848722891566265</v>
       </c>
       <c r="B208" s="0">
-        <v>0.018649725808813876</v>
+        <v>0.019312763093354713</v>
       </c>
       <c r="C208" s="0">
-        <v>1.3707284915418809</v>
+        <v>1.3228476386866694</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0">
-        <v>0.18247196787148592</v>
+        <v>0.19944610441767069</v>
       </c>
       <c r="B209" s="0">
-        <v>0.018860339480032594</v>
+        <v>0.019542968733989124</v>
       </c>
       <c r="C209" s="0">
-        <v>1.4018629213277134</v>
+        <v>1.3545719391215427</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0">
-        <v>0.18334923694779115</v>
+        <v>0.20040497991967873</v>
       </c>
       <c r="B210" s="0">
-        <v>0.019070953151251312</v>
+        <v>0.019773174374623542</v>
       </c>
       <c r="C210" s="0">
-        <v>1.4333469818864071</v>
+        <v>1.3866721487240912</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0">
-        <v>0.18422650602409638</v>
+        <v>0.20136385542168675</v>
       </c>
       <c r="B211" s="0">
-        <v>0.019281566822470037</v>
+        <v>0.020003380015257945</v>
       </c>
       <c r="C211" s="0">
-        <v>1.465180673217962</v>
+        <v>1.4191482674943112</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0">
-        <v>0.1851037751004016</v>
+        <v>0.20232273092369479</v>
       </c>
       <c r="B212" s="0">
-        <v>0.019492180493688754</v>
+        <v>0.020233585655892363</v>
       </c>
       <c r="C212" s="0">
-        <v>1.4973639953223763</v>
+        <v>1.4520002954322069</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0">
-        <v>0.18598104417670683</v>
+        <v>0.20328160642570281</v>
       </c>
       <c r="B213" s="0">
-        <v>0.019702794164907472</v>
+        <v>0.020463791296526767</v>
       </c>
       <c r="C213" s="0">
-        <v>1.5298969481996521</v>
+        <v>1.4852282325377748</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0">
-        <v>0.18685831325301205</v>
+        <v>0.20424048192771083</v>
       </c>
       <c r="B214" s="0">
-        <v>0.01991340783612619</v>
+        <v>0.020693996937161178</v>
       </c>
       <c r="C214" s="0">
-        <v>1.5627795318497877</v>
+        <v>1.5188320788110179</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0">
-        <v>0.18773558232931725</v>
+        <v>0.20519935742971887</v>
       </c>
       <c r="B215" s="0">
-        <v>0.020124021507344901</v>
+        <v>0.020924202577795596</v>
       </c>
       <c r="C215" s="0">
-        <v>1.5960117462727827</v>
+        <v>1.5528118342519357</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0">
-        <v>0.18861285140562248</v>
+        <v>0.20615823293172689</v>
       </c>
       <c r="B216" s="0">
-        <v>0.020334635178563619</v>
+        <v>0.021154408218429999</v>
       </c>
       <c r="C216" s="0">
-        <v>1.6295935914686401</v>
+        <v>1.5871674988605253</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0">
-        <v>0.18949012048192771</v>
+        <v>0.20711710843373493</v>
       </c>
       <c r="B217" s="0">
-        <v>0.020545248849782337</v>
+        <v>0.021384613859064417</v>
       </c>
       <c r="C217" s="0">
-        <v>1.6635250674373576</v>
+        <v>1.6218990726367906</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0">
-        <v>0.19036738955823293</v>
+        <v>0.20807598393574298</v>
       </c>
       <c r="B218" s="0">
-        <v>0.020755862521001055</v>
+        <v>0.021614819499698828</v>
       </c>
       <c r="C218" s="0">
-        <v>1.6978061741789357</v>
+        <v>1.657006555580729</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0">
-        <v>0.19124465863453816</v>
+        <v>0.20903485943775102</v>
       </c>
       <c r="B219" s="0">
-        <v>0.020966476192219773</v>
+        <v>0.021845025140333246</v>
       </c>
       <c r="C219" s="0">
-        <v>1.7324369116933749</v>
+        <v>1.6924899476923425</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0">
-        <v>0.19212192771084338</v>
+        <v>0.20999373493975904</v>
       </c>
       <c r="B220" s="0">
-        <v>0.02117708986343849</v>
+        <v>0.022075230780967649</v>
       </c>
       <c r="C220" s="0">
-        <v>1.767417279980674</v>
+        <v>1.7283492489716277</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0">
-        <v>0.19299919678714858</v>
+        <v>0.21095261044176708</v>
       </c>
       <c r="B221" s="0">
-        <v>0.021387703534657201</v>
+        <v>0.022305436421602067</v>
       </c>
       <c r="C221" s="0">
-        <v>1.8027472790408328</v>
+        <v>1.7645844594185887</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0">
-        <v>0.19387646586345381</v>
+        <v>0.2119114859437751</v>
       </c>
       <c r="B222" s="0">
-        <v>0.021598317205875919</v>
+        <v>0.022535642062236471</v>
       </c>
       <c r="C222" s="0">
-        <v>1.8384269088738538</v>
+        <v>1.8011955790332215</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0">
-        <v>0.19475373493975903</v>
+        <v>0.21287036144578314</v>
       </c>
       <c r="B223" s="0">
-        <v>0.021808930877094637</v>
+        <v>0.022765847702870889</v>
       </c>
       <c r="C223" s="0">
-        <v>1.8744561694797348</v>
+        <v>1.8381826078155308</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0">
-        <v>0.19563100401606426</v>
+        <v>0.21382923694779116</v>
       </c>
       <c r="B224" s="0">
-        <v>0.022019544548313355</v>
+        <v>0.0229960533435053</v>
       </c>
       <c r="C224" s="0">
-        <v>1.9108350608584765</v>
+        <v>1.8755455457655126</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0">
-        <v>0.19650827309236948</v>
+        <v>0.21478811244979917</v>
       </c>
       <c r="B225" s="0">
-        <v>0.022230158219532073</v>
+        <v>0.023226258984139703</v>
       </c>
       <c r="C225" s="0">
-        <v>1.9475635830100795</v>
+        <v>1.9132843928831667</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0">
-        <v>0.19738554216867471</v>
+        <v>0.21574698795180722</v>
       </c>
       <c r="B226" s="0">
-        <v>0.022440771890750791</v>
+        <v>0.023456464624774121</v>
       </c>
       <c r="C226" s="0">
-        <v>1.9846417359345423</v>
+        <v>1.9513991491684977</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0">
-        <v>0.19826281124497994</v>
+        <v>0.21670586345381526</v>
       </c>
       <c r="B227" s="0">
-        <v>0.022651385561969516</v>
+        <v>0.023686670265408532</v>
       </c>
       <c r="C227" s="0">
-        <v>2.022069519631867</v>
+        <v>1.9898898146215012</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0">
-        <v>0.19914008032128513</v>
+        <v>0.21766473895582331</v>
       </c>
       <c r="B228" s="0">
-        <v>0.022861999233188227</v>
+        <v>0.02391687590604295</v>
       </c>
       <c r="C228" s="0">
-        <v>2.0598469341020507</v>
+        <v>2.0287563892421798</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0">
-        <v>0.20001734939759036</v>
+        <v>0.21862361445783132</v>
       </c>
       <c r="B229" s="0">
-        <v>0.023072612904406944</v>
+        <v>0.024147081546677354</v>
       </c>
       <c r="C229" s="0">
-        <v>2.0979739793450953</v>
+        <v>2.0679988730305294</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0">
-        <v>0.20089461847389559</v>
+        <v>0.21958248995983937</v>
       </c>
       <c r="B230" s="0">
-        <v>0.023283226575625662</v>
+        <v>0.024377287187311771</v>
       </c>
       <c r="C230" s="0">
-        <v>2.1364506553610005</v>
+        <v>2.1076172659865562</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0">
-        <v>0.20177188755020081</v>
+        <v>0.22054136546184738</v>
       </c>
       <c r="B231" s="0">
-        <v>0.02349384024684438</v>
+        <v>0.024607492827946182</v>
       </c>
       <c r="C231" s="0">
-        <v>2.1752769621497672</v>
+        <v>2.1476115681102557</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0">
-        <v>0.20264915662650604</v>
+        <v>0.22150024096385543</v>
       </c>
       <c r="B232" s="0">
-        <v>0.023704453918063098</v>
+        <v>0.024837698468580593</v>
       </c>
       <c r="C232" s="0">
-        <v>2.2144528997113935</v>
+        <v>2.1879817794016288</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0">
-        <v>0.20352642570281124</v>
+        <v>0.22245911646586344</v>
       </c>
       <c r="B233" s="0">
-        <v>0.023915067589281809</v>
+        <v>0.025067904109215004</v>
       </c>
       <c r="C233" s="0">
-        <v>2.2539784680458794</v>
+        <v>2.228727899860675</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0">
-        <v>0.20440369477911646</v>
+        <v>0.22341799196787149</v>
       </c>
       <c r="B234" s="0">
-        <v>0.024125681260500527</v>
+        <v>0.025298109749849414</v>
       </c>
       <c r="C234" s="0">
-        <v>2.2938536671532277</v>
+        <v>2.2698499294873957</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0">
-        <v>0.20528096385542166</v>
+        <v>0.22437686746987953</v>
       </c>
       <c r="B235" s="0">
-        <v>0.024336294931719238</v>
+        <v>0.025528315390483832</v>
       </c>
       <c r="C235" s="0">
-        <v>2.3340784970334347</v>
+        <v>2.3113478682817923</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0">
-        <v>0.20615823293172689</v>
+        <v>0.22533574297188755</v>
       </c>
       <c r="B236" s="0">
-        <v>0.024546908602937956</v>
+        <v>0.025758521031118236</v>
       </c>
       <c r="C236" s="0">
-        <v>2.3746529576865045</v>
+        <v>2.3532217162438593</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0">
-        <v>0.20703550200803211</v>
+        <v>0.22629461847389559</v>
       </c>
       <c r="B237" s="0">
-        <v>0.024757522274156674</v>
+        <v>0.025988726671752654</v>
       </c>
       <c r="C237" s="0">
-        <v>2.415577049112434</v>
+        <v>2.3954714733736027</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0">
-        <v>0.20791277108433734</v>
+        <v>0.22725349397590361</v>
       </c>
       <c r="B238" s="0">
-        <v>0.024968135945375392</v>
+        <v>0.026218932312387058</v>
       </c>
       <c r="C238" s="0">
-        <v>2.456850771311224</v>
+        <v>2.4380971396710178</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0">
-        <v>0.20879004016064256</v>
+        <v>0.22821236947791165</v>
       </c>
       <c r="B239" s="0">
-        <v>0.025178749616594109</v>
+        <v>0.026449137953021475</v>
       </c>
       <c r="C239" s="0">
-        <v>2.4984741242828754</v>
+        <v>2.4810987151361097</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0">
-        <v>0.20966730923694779</v>
+        <v>0.22917124497991967</v>
       </c>
       <c r="B240" s="0">
-        <v>0.025389363287812827</v>
+        <v>0.026679343593655886</v>
       </c>
       <c r="C240" s="0">
-        <v>2.5404471080273869</v>
+        <v>2.5244761997688743</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0">
-        <v>0.21054457831325299</v>
+        <v>0.23013012048192771</v>
       </c>
       <c r="B241" s="0">
-        <v>0.025599976959031538</v>
+        <v>0.026909549234290297</v>
       </c>
       <c r="C241" s="0">
-        <v>2.5827697225447572</v>
+        <v>2.5682295935693116</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0">
-        <v>0.21142184738955822</v>
+        <v>0.23108899598393573</v>
       </c>
       <c r="B242" s="0">
-        <v>0.025810590630250263</v>
+        <v>0.027139754874924708</v>
       </c>
       <c r="C242" s="0">
-        <v>2.6254419678349912</v>
+        <v>2.6123588965374238</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0">
-        <v>0.21229911646586344</v>
+        <v>0.23204787148594378</v>
       </c>
       <c r="B243" s="0">
-        <v>0.026021204301468981</v>
+        <v>0.027369960515559119</v>
       </c>
       <c r="C243" s="0">
-        <v>2.6684638438980852</v>
+        <v>2.6568641086732101</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0">
-        <v>0.21317638554216867</v>
+        <v>0.23300674698795182</v>
       </c>
       <c r="B244" s="0">
-        <v>0.026231817972687699</v>
+        <v>0.027600166156193536</v>
       </c>
       <c r="C244" s="0">
-        <v>2.7118353507340389</v>
+        <v>2.7017452299766713</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0">
-        <v>0.21405365461847389</v>
+        <v>0.23396562248995986</v>
       </c>
       <c r="B245" s="0">
-        <v>0.026442431643906417</v>
+        <v>0.027830371796827947</v>
       </c>
       <c r="C245" s="0">
-        <v>2.7555564883428536</v>
+        <v>2.7470022604478044</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0">
-        <v>0.21493092369477912</v>
+        <v>0.23492449799196788</v>
       </c>
       <c r="B246" s="0">
-        <v>0.026653045315125135</v>
+        <v>0.028060577437462358</v>
       </c>
       <c r="C246" s="0">
-        <v>2.7996272567245293</v>
+        <v>2.7926352000866124</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0">
-        <v>0.21580819277108435</v>
+        <v>0.2358833734939759</v>
       </c>
       <c r="B247" s="0">
-        <v>0.026863658986343853</v>
+        <v>0.028290783078096762</v>
       </c>
       <c r="C247" s="0">
-        <v>2.8440476558790646</v>
+        <v>2.8386440488930926</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0">
-        <v>0.21668546184738954</v>
+        <v>0.23684224899598394</v>
       </c>
       <c r="B248" s="0">
-        <v>0.027074272657562563</v>
+        <v>0.028520988718731179</v>
       </c>
       <c r="C248" s="0">
-        <v>2.88881768580646</v>
+        <v>2.8850288068672496</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0">
-        <v>0.21756273092369477</v>
+        <v>0.23780112449799196</v>
       </c>
       <c r="B249" s="0">
-        <v>0.027284886328781281</v>
+        <v>0.02875119435936559</v>
       </c>
       <c r="C249" s="0">
-        <v>2.9339373465067169</v>
+        <v>2.9317894740090789</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0">
-        <v>0.21844</v>
+        <v>0.23876</v>
       </c>
       <c r="B250" s="0">
-        <v>0.027495499999999999</v>
+        <v>0.028981400000000001</v>
       </c>
       <c r="C250" s="0">
-        <v>2.9794066379798343</v>
+        <v>2.9789260503185817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIxed missing maelstrom files
</commit_message>
<xml_diff>
--- a/REGEN/Contour_Maelstrom.xlsx
+++ b/REGEN/Contour_Maelstrom.xlsx
@@ -59,7 +59,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="true"/>
+    <col min="1" max="1" width="15.5546875" customWidth="true"/>
     <col min="2" max="2" width="13.5546875" customWidth="true"/>
     <col min="3" max="3" width="11.5546875" customWidth="true"/>
   </cols>
@@ -72,2746 +72,2746 @@
         <v>0.043179999999999996</v>
       </c>
       <c r="C1" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.00095887550200803213</v>
+        <v>0.0008772690763052209</v>
       </c>
       <c r="B2" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C2" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.0019177510040160643</v>
+        <v>0.0017545381526104418</v>
       </c>
       <c r="B3" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C3" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>0.0028766265060240965</v>
+        <v>0.0026318072289156628</v>
       </c>
       <c r="B4" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C4" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>0.0038355020080321285</v>
+        <v>0.0035090763052208836</v>
       </c>
       <c r="B5" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C5" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0.0047943775100401601</v>
+        <v>0.0043863453815261048</v>
       </c>
       <c r="B6" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C6" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0.005753253012048193</v>
+        <v>0.0052636144578313256</v>
       </c>
       <c r="B7" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C7" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0.0067121285140562242</v>
+        <v>0.0061408835341365464</v>
       </c>
       <c r="B8" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C8" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0.0076710040160642571</v>
+        <v>0.0070181526104417672</v>
       </c>
       <c r="B9" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C9" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0.0086298795180722882</v>
+        <v>0.0078954216867469871</v>
       </c>
       <c r="B10" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C10" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.0095887550200803202</v>
+        <v>0.0087726907630522096</v>
       </c>
       <c r="B11" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C11" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0.010547630522088354</v>
+        <v>0.0096499598393574287</v>
       </c>
       <c r="B12" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C12" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.011506506024096386</v>
+        <v>0.010527228915662651</v>
       </c>
       <c r="B13" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C13" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0.012465381526104418</v>
+        <v>0.01140449799196787</v>
       </c>
       <c r="B14" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C14" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0.013424257028112448</v>
+        <v>0.012281767068273093</v>
       </c>
       <c r="B15" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C15" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0.014383132530120482</v>
+        <v>0.013159036144578312</v>
       </c>
       <c r="B16" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C16" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.015342008032128514</v>
+        <v>0.014036305220883534</v>
       </c>
       <c r="B17" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C17" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0.016300883534136546</v>
+        <v>0.014913574297188755</v>
       </c>
       <c r="B18" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C18" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0.017259759036144576</v>
+        <v>0.015790843373493974</v>
       </c>
       <c r="B19" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C19" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>0.01821863453815261</v>
+        <v>0.016668112449799197</v>
       </c>
       <c r="B20" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C20" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>0.01917751004016064</v>
+        <v>0.017545381526104419</v>
       </c>
       <c r="B21" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C21" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>0.020136385542168674</v>
+        <v>0.018422650602409638</v>
       </c>
       <c r="B22" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C22" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.021095261044176708</v>
+        <v>0.019299919678714857</v>
       </c>
       <c r="B23" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C23" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0.022054136546184738</v>
+        <v>0.02017718875502008</v>
       </c>
       <c r="B24" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C24" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>0.023013012048192772</v>
+        <v>0.021054457831325302</v>
       </c>
       <c r="B25" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C25" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>0.023971887550200806</v>
+        <v>0.021931726907630525</v>
       </c>
       <c r="B26" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C26" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>0.024930763052208836</v>
+        <v>0.022808995983935741</v>
       </c>
       <c r="B27" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C27" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>0.025889638554216866</v>
+        <v>0.023686265060240963</v>
       </c>
       <c r="B28" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C28" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>0.026848514056224897</v>
+        <v>0.024563534136546186</v>
       </c>
       <c r="B29" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C29" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0.027807389558232931</v>
+        <v>0.025440803212851405</v>
       </c>
       <c r="B30" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C30" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>0.028766265060240964</v>
+        <v>0.026318072289156624</v>
       </c>
       <c r="B31" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C31" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>0.029725140562248994</v>
+        <v>0.027195341365461846</v>
       </c>
       <c r="B32" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C32" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>0.030684016064257028</v>
+        <v>0.028072610441767069</v>
       </c>
       <c r="B33" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C33" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>0.031642891566265062</v>
+        <v>0.028949879518072288</v>
       </c>
       <c r="B34" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C34" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>0.032601767068273092</v>
+        <v>0.02982714859437751</v>
       </c>
       <c r="B35" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C35" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>0.033560642570281123</v>
+        <v>0.030704417670682729</v>
       </c>
       <c r="B36" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C36" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>0.034519518072289153</v>
+        <v>0.031581686746987948</v>
       </c>
       <c r="B37" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C37" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>0.03547839357429719</v>
+        <v>0.032458955823293167</v>
       </c>
       <c r="B38" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C38" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>0.03643726907630522</v>
+        <v>0.033336224899598394</v>
       </c>
       <c r="B39" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C39" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>0.037396144578313258</v>
+        <v>0.034213493975903612</v>
       </c>
       <c r="B40" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C40" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>0.038355020080321281</v>
+        <v>0.035090763052208838</v>
       </c>
       <c r="B41" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C41" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0.039313895582329318</v>
+        <v>0.035968032128514058</v>
       </c>
       <c r="B42" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C42" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>0.040272771084337349</v>
+        <v>0.036845301204819277</v>
       </c>
       <c r="B43" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C43" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>0.041231646586345379</v>
+        <v>0.037722570281124496</v>
       </c>
       <c r="B44" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C44" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>0.042190522088353416</v>
+        <v>0.038599839357429715</v>
       </c>
       <c r="B45" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C45" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>0.043149397590361446</v>
+        <v>0.039477108433734941</v>
       </c>
       <c r="B46" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C46" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>0.044108273092369477</v>
+        <v>0.04035437751004016</v>
       </c>
       <c r="B47" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C47" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0.045067148594377507</v>
+        <v>0.041231646586345379</v>
       </c>
       <c r="B48" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C48" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>0.046026024096385544</v>
+        <v>0.042108915662650605</v>
       </c>
       <c r="B49" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C49" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>0.046984899598393574</v>
+        <v>0.042986184738955824</v>
       </c>
       <c r="B50" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C50" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0.047943775100401612</v>
+        <v>0.04386345381526105</v>
       </c>
       <c r="B51" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C51" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0.048902650602409635</v>
+        <v>0.044740722891566262</v>
       </c>
       <c r="B52" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C52" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0.049861526104417672</v>
+        <v>0.045617991967871481</v>
       </c>
       <c r="B53" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0.050820401606425702</v>
+        <v>0.046495261044176707</v>
       </c>
       <c r="B54" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C54" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0.051779277108433733</v>
+        <v>0.047372530120481926</v>
       </c>
       <c r="B55" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0.05273815261044177</v>
+        <v>0.048249799196787145</v>
       </c>
       <c r="B56" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C56" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0.053697028112449793</v>
+        <v>0.049127068273092371</v>
       </c>
       <c r="B57" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C57" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0.054655903614457831</v>
+        <v>0.05000433734939759</v>
       </c>
       <c r="B58" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C58" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0.055614779116465861</v>
+        <v>0.050881606425702809</v>
       </c>
       <c r="B59" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0.056573654618473898</v>
+        <v>0.051758875502008028</v>
       </c>
       <c r="B60" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C60" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
-        <v>0.057532530120481928</v>
+        <v>0.052636144578313247</v>
       </c>
       <c r="B61" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C61" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
-        <v>0.058491405622489966</v>
+        <v>0.053513413654618473</v>
       </c>
       <c r="B62" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C62" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
-        <v>0.059450281124497989</v>
+        <v>0.054390682730923692</v>
       </c>
       <c r="B63" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C63" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
-        <v>0.060409156626506026</v>
+        <v>0.055267951807228918</v>
       </c>
       <c r="B64" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C64" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
-        <v>0.061368032128514057</v>
+        <v>0.056145220883534137</v>
       </c>
       <c r="B65" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C65" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
-        <v>0.062326907630522087</v>
+        <v>0.057022489959839356</v>
       </c>
       <c r="B66" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C66" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>0.063285783132530124</v>
+        <v>0.057899759036144576</v>
       </c>
       <c r="B67" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C67" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
-        <v>0.064244658634538154</v>
+        <v>0.058777028112449795</v>
       </c>
       <c r="B68" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C68" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
-        <v>0.065203534136546185</v>
+        <v>0.059654297188755021</v>
       </c>
       <c r="B69" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C69" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
-        <v>0.066162409638554229</v>
+        <v>0.06053156626506024</v>
       </c>
       <c r="B70" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C70" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
-        <v>0.067121285140562245</v>
+        <v>0.061408835341365459</v>
       </c>
       <c r="B71" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C71" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
-        <v>0.068080160642570276</v>
+        <v>0.062286104417670685</v>
       </c>
       <c r="B72" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C72" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
-        <v>0.069039036144578306</v>
+        <v>0.063163373493975897</v>
       </c>
       <c r="B73" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C73" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
-        <v>0.06999791164658635</v>
+        <v>0.064040642570281123</v>
       </c>
       <c r="B74" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C74" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
-        <v>0.07095678714859438</v>
+        <v>0.064917911646586335</v>
       </c>
       <c r="B75" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C75" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
-        <v>0.07191566265060241</v>
+        <v>0.065795180722891561</v>
       </c>
       <c r="B76" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C76" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
-        <v>0.072874538152610441</v>
+        <v>0.066672449799196787</v>
       </c>
       <c r="B77" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C77" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
-        <v>0.073833413654618471</v>
+        <v>0.067549718875502013</v>
       </c>
       <c r="B78" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C78" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
-        <v>0.074792289156626515</v>
+        <v>0.068426987951807225</v>
       </c>
       <c r="B79" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C79" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
-        <v>0.075751164658634546</v>
+        <v>0.069304257028112451</v>
       </c>
       <c r="B80" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C80" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
-        <v>0.076710040160642562</v>
+        <v>0.070181526104417677</v>
       </c>
       <c r="B81" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C81" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
-        <v>0.077668915662650592</v>
+        <v>0.071058795180722889</v>
       </c>
       <c r="B82" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C82" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
-        <v>0.078627791164658636</v>
+        <v>0.071936064257028115</v>
       </c>
       <c r="B83" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C83" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
-        <v>0.079586666666666667</v>
+        <v>0.072813333333333341</v>
       </c>
       <c r="B84" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C84" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
-        <v>0.080545542168674697</v>
+        <v>0.073690602409638553</v>
       </c>
       <c r="B85" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C85" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
-        <v>0.081504417670682727</v>
+        <v>0.074567871485943765</v>
       </c>
       <c r="B86" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C86" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
-        <v>0.082463293172690758</v>
+        <v>0.075445140562248991</v>
       </c>
       <c r="B87" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C87" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
-        <v>0.083422168674698802</v>
+        <v>0.076322409638554203</v>
       </c>
       <c r="B88" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C88" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
-        <v>0.084381044176706832</v>
+        <v>0.077199678714859429</v>
       </c>
       <c r="B89" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C89" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
-        <v>0.085339919678714862</v>
+        <v>0.078076947791164655</v>
       </c>
       <c r="B90" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C90" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
-        <v>0.086298795180722893</v>
+        <v>0.078954216867469881</v>
       </c>
       <c r="B91" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C91" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
-        <v>0.087257670682730923</v>
+        <v>0.079831485943775093</v>
       </c>
       <c r="B92" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C92" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
-        <v>0.088216546184738953</v>
+        <v>0.08070875502008032</v>
       </c>
       <c r="B93" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C93" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0">
-        <v>0.089175421686746983</v>
+        <v>0.081586024096385546</v>
       </c>
       <c r="B94" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C94" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0">
-        <v>0.090134297188755014</v>
+        <v>0.082463293172690758</v>
       </c>
       <c r="B95" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C95" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0">
-        <v>0.091093172690763058</v>
+        <v>0.083340562248995984</v>
       </c>
       <c r="B96" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C96" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0">
-        <v>0.092052048192771088</v>
+        <v>0.08421783132530121</v>
       </c>
       <c r="B97" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C97" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0">
-        <v>0.093010923694779119</v>
+        <v>0.085095100401606422</v>
       </c>
       <c r="B98" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C98" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0">
-        <v>0.093969799196787149</v>
+        <v>0.085972369477911648</v>
       </c>
       <c r="B99" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C99" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0">
-        <v>0.094928674698795179</v>
+        <v>0.086849638554216874</v>
       </c>
       <c r="B100" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C100" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0">
-        <v>0.095887550200803223</v>
+        <v>0.0877269076305221</v>
       </c>
       <c r="B101" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C101" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0">
-        <v>0.096846425702811254</v>
+        <v>0.088604176706827298</v>
       </c>
       <c r="B102" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C102" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0">
-        <v>0.09780530120481927</v>
+        <v>0.089481445783132524</v>
       </c>
       <c r="B103" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C103" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0">
-        <v>0.0987641767068273</v>
+        <v>0.09035871485943775</v>
       </c>
       <c r="B104" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C104" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0">
-        <v>0.099723052208835344</v>
+        <v>0.091235983935742962</v>
       </c>
       <c r="B105" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C105" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0">
-        <v>0.10068192771084337</v>
+        <v>0.092113253012048188</v>
       </c>
       <c r="B106" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C106" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0">
-        <v>0.1016408032128514</v>
+        <v>0.092990522088353414</v>
       </c>
       <c r="B107" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C107" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0">
-        <v>0.10259967871485944</v>
+        <v>0.093867791164658626</v>
       </c>
       <c r="B108" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C108" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0">
-        <v>0.10355855421686747</v>
+        <v>0.094745060240963852</v>
       </c>
       <c r="B109" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C109" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0">
-        <v>0.10451742971887551</v>
+        <v>0.095622329317269078</v>
       </c>
       <c r="B110" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C110" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0">
-        <v>0.10547630522088354</v>
+        <v>0.09649959839357429</v>
       </c>
       <c r="B111" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C111" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0">
-        <v>0.10643518072289157</v>
+        <v>0.097376867469879516</v>
       </c>
       <c r="B112" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C112" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0">
-        <v>0.10739405622489959</v>
+        <v>0.098254136546184742</v>
       </c>
       <c r="B113" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C113" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0">
-        <v>0.10835293172690763</v>
+        <v>0.099131405622489968</v>
       </c>
       <c r="B114" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C114" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0">
-        <v>0.10931180722891566</v>
+        <v>0.10000867469879518</v>
       </c>
       <c r="B115" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C115" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0">
-        <v>0.11027068273092369</v>
+        <v>0.10088594377510041</v>
       </c>
       <c r="B116" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C116" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0">
-        <v>0.11122955823293172</v>
+        <v>0.10176321285140562</v>
       </c>
       <c r="B117" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C117" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0">
-        <v>0.11218843373493977</v>
+        <v>0.10264048192771083</v>
       </c>
       <c r="B118" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C118" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0">
-        <v>0.1131473092369478</v>
+        <v>0.10351775100401606</v>
       </c>
       <c r="B119" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C119" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0">
-        <v>0.11410618473895583</v>
+        <v>0.10439502008032128</v>
       </c>
       <c r="B120" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C120" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0">
-        <v>0.11506506024096386</v>
+        <v>0.10527228915662649</v>
       </c>
       <c r="B121" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C121" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0">
-        <v>0.11602393574297189</v>
+        <v>0.10614955823293172</v>
       </c>
       <c r="B122" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C122" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0">
-        <v>0.11698281124497993</v>
+        <v>0.10702682730923695</v>
       </c>
       <c r="B123" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C123" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0">
-        <v>0.11794168674698795</v>
+        <v>0.10790409638554217</v>
       </c>
       <c r="B124" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C124" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0">
-        <v>0.11890056224899598</v>
+        <v>0.10878136546184738</v>
       </c>
       <c r="B125" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C125" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0">
-        <v>0.11985943775100401</v>
+        <v>0.10965863453815261</v>
       </c>
       <c r="B126" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C126" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0">
-        <v>0.12081831325301205</v>
+        <v>0.11053590361445784</v>
       </c>
       <c r="B127" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C127" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0">
-        <v>0.12177718875502008</v>
+        <v>0.11141317269076305</v>
       </c>
       <c r="B128" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C128" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0">
-        <v>0.12273606425702811</v>
+        <v>0.11229044176706827</v>
       </c>
       <c r="B129" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C129" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0">
-        <v>0.12369493975903614</v>
+        <v>0.1131677108433735</v>
       </c>
       <c r="B130" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C130" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0">
-        <v>0.12465381526104417</v>
+        <v>0.11404497991967871</v>
       </c>
       <c r="B131" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C131" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0">
-        <v>0.1256126907630522</v>
+        <v>0.11492224899598394</v>
       </c>
       <c r="B132" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C132" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0">
-        <v>0.12657156626506025</v>
+        <v>0.11579951807228915</v>
       </c>
       <c r="B133" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C133" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0">
-        <v>0.12753044176706827</v>
+        <v>0.11667678714859436</v>
       </c>
       <c r="B134" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C134" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0">
-        <v>0.12848931726907631</v>
+        <v>0.11755405622489959</v>
       </c>
       <c r="B135" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C135" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0">
-        <v>0.12944819277108432</v>
+        <v>0.11843132530120482</v>
       </c>
       <c r="B136" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C136" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0">
-        <v>0.13040706827309237</v>
+        <v>0.11930859437751004</v>
       </c>
       <c r="B137" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C137" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0">
-        <v>0.13136594377510041</v>
+        <v>0.12018586345381525</v>
       </c>
       <c r="B138" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C138" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0">
-        <v>0.13232481927710846</v>
+        <v>0.12106313253012048</v>
       </c>
       <c r="B139" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C139" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0">
-        <v>0.13328369477911647</v>
+        <v>0.12194040160642571</v>
       </c>
       <c r="B140" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C140" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0">
-        <v>0.13424257028112449</v>
+        <v>0.12281767068273092</v>
       </c>
       <c r="B141" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C141" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0">
-        <v>0.13520144578313253</v>
+        <v>0.12369493975903614</v>
       </c>
       <c r="B142" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C142" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0">
-        <v>0.13616032128514055</v>
+        <v>0.12457220883534137</v>
       </c>
       <c r="B143" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C143" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0">
-        <v>0.1371191967871486</v>
+        <v>0.12544947791164657</v>
       </c>
       <c r="B144" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C144" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0">
-        <v>0.13807807228915661</v>
+        <v>0.12632674698795179</v>
       </c>
       <c r="B145" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C145" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0">
-        <v>0.13903694779116466</v>
+        <v>0.12720401606425702</v>
       </c>
       <c r="B146" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C146" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0">
-        <v>0.1399958232931727</v>
+        <v>0.12808128514056225</v>
       </c>
       <c r="B147" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C147" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0">
-        <v>0.14095469879518074</v>
+        <v>0.12895855421686747</v>
       </c>
       <c r="B148" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C148" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0">
-        <v>0.14191357429718876</v>
+        <v>0.12983582329317267</v>
       </c>
       <c r="B149" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C149" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0">
-        <v>0.14287244979919678</v>
+        <v>0.1307130923694779</v>
       </c>
       <c r="B150" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C150" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0">
-        <v>0.14383132530120482</v>
+        <v>0.13159036144578312</v>
       </c>
       <c r="B151" s="0">
         <v>0.043179999999999996</v>
       </c>
       <c r="C151" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3480451087897176</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0">
-        <v>0.14479020080321284</v>
+        <v>0.13246763052208835</v>
       </c>
       <c r="B152" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.043179177500336327</v>
       </c>
       <c r="C152" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3477651779388937</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0">
-        <v>0.14574907630522088</v>
+        <v>0.13334489959839357</v>
       </c>
       <c r="B153" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.043138827483513054</v>
       </c>
       <c r="C153" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.3340389359190654</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0">
-        <v>0.1467079518072289</v>
+        <v>0.1342221686746988</v>
       </c>
       <c r="B154" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.043037209692649056</v>
       </c>
       <c r="C154" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.2995275177448633</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0">
-        <v>0.14766682730923694</v>
+        <v>0.13509943775100403</v>
       </c>
       <c r="B155" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.042872817081216472</v>
       </c>
       <c r="C155" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.2438688654090022</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0">
-        <v>0.14862570281124499</v>
+        <v>0.13597670682730922</v>
       </c>
       <c r="B156" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.04264310458260305</v>
       </c>
       <c r="C156" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.1664515434123128</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0">
-        <v>0.14958457831325303</v>
+        <v>0.13685397590361445</v>
       </c>
       <c r="B157" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.042344278692853808</v>
       </c>
       <c r="C157" s="0">
-        <v>6.6128135255224567</v>
+        <v>7.0663641874026189</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0">
-        <v>0.15054345381526105</v>
+        <v>0.13773124497991968</v>
       </c>
       <c r="B158" s="0">
-        <v>0.043179999999999996</v>
+        <v>0.041970948727219508</v>
       </c>
       <c r="C158" s="0">
-        <v>6.6128135255224567</v>
+        <v>6.9423117208563223</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0">
-        <v>0.15150232931726909</v>
+        <v>0.1386085140562249</v>
       </c>
       <c r="B159" s="0">
-        <v>0.043166394565478709</v>
+        <v>0.041515555914270363</v>
       </c>
       <c r="C159" s="0">
-        <v>6.6086469656694868</v>
+        <v>6.7924781986975518</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0">
-        <v>0.15246120481927711</v>
+        <v>0.13948578313253013</v>
       </c>
       <c r="B160" s="0">
-        <v>0.043085478963667503</v>
+        <v>0.040967415504208113</v>
       </c>
       <c r="C160" s="0">
-        <v>6.58389430967362</v>
+        <v>6.614296680126035</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0">
-        <v>0.15342008032128512</v>
+        <v>0.14036305220883535</v>
       </c>
       <c r="B161" s="0">
-        <v>0.042930409964303105</v>
+        <v>0.040311025964482994</v>
       </c>
       <c r="C161" s="0">
-        <v>6.5365873904226328</v>
+        <v>6.4040430239947961</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0">
-        <v>0.15437895582329317</v>
+        <v>0.14124032128514055</v>
       </c>
       <c r="B162" s="0">
-        <v>0.042698364546790608</v>
+        <v>0.039522845625481542</v>
       </c>
       <c r="C162" s="0">
-        <v>6.466115856432249</v>
+        <v>6.1560614991563316</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0">
-        <v>0.15533783132530118</v>
+        <v>0.14211759036144578</v>
       </c>
       <c r="B163" s="0">
-        <v>0.04238484236185508</v>
+        <v>0.038646015850478291</v>
       </c>
       <c r="C163" s="0">
-        <v>6.3715067091828424</v>
+        <v>5.8859422006254709</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0">
-        <v>0.15629670682730923</v>
+        <v>0.14299485943775101</v>
       </c>
       <c r="B164" s="0">
-        <v>0.041983183327508354</v>
+        <v>0.037768746774173065</v>
       </c>
       <c r="C164" s="0">
-        <v>6.2513200049013458</v>
+        <v>5.6217520473418068</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0">
-        <v>0.15725558232931727</v>
+        <v>0.14387212851405623</v>
       </c>
       <c r="B165" s="0">
-        <v>0.041483740146659717</v>
+        <v>0.036891477697867839</v>
       </c>
       <c r="C165" s="0">
-        <v>6.1034699486384767</v>
+        <v>5.3636278908310029</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0">
-        <v>0.15821445783132532</v>
+        <v>0.14474939759036146</v>
       </c>
       <c r="B166" s="0">
-        <v>0.040872424322912</v>
+        <v>0.036014208621562613</v>
       </c>
       <c r="C166" s="0">
-        <v>5.9249105354508975</v>
+        <v>5.1115697310930637</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0">
-        <v>0.15917333333333333</v>
+        <v>0.14562666666666668</v>
       </c>
       <c r="B167" s="0">
-        <v>0.04012799382996244</v>
+        <v>0.035136939545257387</v>
       </c>
       <c r="C167" s="0">
-        <v>5.7110491306598821</v>
+        <v>4.8655775681279847</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0">
-        <v>0.16013220883534138</v>
+        <v>0.14650393574297191</v>
       </c>
       <c r="B168" s="0">
-        <v>0.039222931329655403</v>
+        <v>0.034259670468952168</v>
       </c>
       <c r="C168" s="0">
-        <v>5.4563358638756201</v>
+        <v>4.6256514019357731</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0">
-        <v>0.16109108433734939</v>
+        <v>0.14738120481927711</v>
       </c>
       <c r="B169" s="0">
-        <v>0.038264055827647386</v>
+        <v>0.03338240139264697</v>
       </c>
       <c r="C169" s="0">
-        <v>5.1928168246791691</v>
+        <v>4.391791232516427</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0">
-        <v>0.16204995983935744</v>
+        <v>0.14825847389558233</v>
       </c>
       <c r="B170" s="0">
-        <v>0.037305180325639342</v>
+        <v>0.032505132316341744</v>
       </c>
       <c r="C170" s="0">
-        <v>4.9358197051047812</v>
+        <v>4.1639970598699376</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0">
-        <v>0.16300883534136545</v>
+        <v>0.14913574297188753</v>
       </c>
       <c r="B171" s="0">
-        <v>0.036346304823631326</v>
+        <v>0.031627863240036545</v>
       </c>
       <c r="C171" s="0">
-        <v>4.6853445051524716</v>
+        <v>3.9422688839963169</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0">
-        <v>0.16396771084337347</v>
+        <v>0.15001301204819276</v>
       </c>
       <c r="B172" s="0">
-        <v>0.035387429321623309</v>
+        <v>0.030750594163731319</v>
       </c>
       <c r="C172" s="0">
-        <v>4.4413912248222323</v>
+        <v>3.7266067048955516</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0">
-        <v>0.16492658634538152</v>
+        <v>0.15089028112449798</v>
       </c>
       <c r="B173" s="0">
-        <v>0.034428553819615265</v>
+        <v>0.029873325087426093</v>
       </c>
       <c r="C173" s="0">
-        <v>4.2039598641140579</v>
+        <v>3.5170105225676491</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0">
-        <v>0.16588546184738956</v>
+        <v>0.15176755020080321</v>
       </c>
       <c r="B174" s="0">
-        <v>0.033469678317607221</v>
+        <v>0.028996056011120867</v>
       </c>
       <c r="C174" s="0">
-        <v>3.9730504230279524</v>
+        <v>3.3134803370126091</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0">
-        <v>0.1668443373493976</v>
+        <v>0.15264481927710841</v>
       </c>
       <c r="B175" s="0">
-        <v>0.032510802815599177</v>
+        <v>0.028118786934815669</v>
       </c>
       <c r="C175" s="0">
-        <v>3.7486629015639181</v>
+        <v>3.1160161482304378</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0">
-        <v>0.16780321285140562</v>
+        <v>0.15352208835341363</v>
       </c>
       <c r="B176" s="0">
-        <v>0.031551927313591161</v>
+        <v>0.027241517858510443</v>
       </c>
       <c r="C176" s="0">
-        <v>3.5307972997219621</v>
+        <v>2.9246179562211232</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0">
-        <v>0.16876208835341366</v>
+        <v>0.15439935742971886</v>
       </c>
       <c r="B177" s="0">
-        <v>0.030593051811583116</v>
+        <v>0.026364248782205217</v>
       </c>
       <c r="C177" s="0">
-        <v>3.3194536175020688</v>
+        <v>2.7392857609846706</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0">
-        <v>0.16972096385542168</v>
+        <v>0.15527662650602409</v>
       </c>
       <c r="B178" s="0">
-        <v>0.0296341763095751</v>
+        <v>0.025486979705899991</v>
       </c>
       <c r="C178" s="0">
-        <v>3.1146318549042533</v>
+        <v>2.5600195625210809</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0">
-        <v>0.17067983935742973</v>
+        <v>0.15615389558232931</v>
       </c>
       <c r="B179" s="0">
-        <v>0.028675300807567056</v>
+        <v>0.024609710629594765</v>
       </c>
       <c r="C179" s="0">
-        <v>2.9163320119285023</v>
+        <v>2.3868193608303532</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0">
-        <v>0.17163871485943774</v>
+        <v>0.15703116465863454</v>
       </c>
       <c r="B180" s="0">
-        <v>0.027716425305559039</v>
+        <v>0.023732441553289539</v>
       </c>
       <c r="C180" s="0">
-        <v>2.7245540885748278</v>
+        <v>2.2196851559124884</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0">
-        <v>0.17259759036144579</v>
+        <v>0.15790843373493976</v>
       </c>
       <c r="B181" s="0">
-        <v>0.026757549803550995</v>
+        <v>0.022855172476984313</v>
       </c>
       <c r="C181" s="0">
-        <v>2.5392980848432183</v>
+        <v>2.0586169477674861</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0">
-        <v>0.17355646586345383</v>
+        <v>0.15878570281124496</v>
       </c>
       <c r="B182" s="0">
-        <v>0.025798674301542951</v>
+        <v>0.021977903400679115</v>
       </c>
       <c r="C182" s="0">
-        <v>2.3605640007336794</v>
+        <v>1.9036147363953513</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0">
-        <v>0.17451534136546185</v>
+        <v>0.15966297188755019</v>
       </c>
       <c r="B183" s="0">
-        <v>0.024839798799534935</v>
+        <v>0.021100634324373889</v>
       </c>
       <c r="C183" s="0">
-        <v>2.1883518362462171</v>
+        <v>1.7546785217960745</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0">
-        <v>0.17547421686746989</v>
+        <v>0.16054024096385541</v>
       </c>
       <c r="B184" s="0">
-        <v>0.02388092329752689</v>
+        <v>0.020223365248068663</v>
       </c>
       <c r="C184" s="0">
-        <v>2.0226615913808192</v>
+        <v>1.6118083039696598</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0">
-        <v>0.17643309236947791</v>
+        <v>0.16141751004016064</v>
       </c>
       <c r="B185" s="0">
-        <v>0.022922047795518874</v>
+        <v>0.019346096171763437</v>
       </c>
       <c r="C185" s="0">
-        <v>1.8634932661374972</v>
+        <v>1.4750040829161075</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0">
-        <v>0.17739196787148595</v>
+        <v>0.16229477911646586</v>
       </c>
       <c r="B186" s="0">
-        <v>0.02196317229351083</v>
+        <v>0.018493455175667396</v>
       </c>
       <c r="C186" s="0">
-        <v>1.7108468605162417</v>
+        <v>1.3478533914019819</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0">
-        <v>0.17835084337349397</v>
+        <v>0.16317204819277109</v>
       </c>
       <c r="B187" s="0">
-        <v>0.021004296791502813</v>
+        <v>0.017796062217276289</v>
       </c>
       <c r="C187" s="0">
-        <v>1.5647223745170609</v>
+        <v>1.2481143273854132</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0">
-        <v>0.17930971887550201</v>
+        <v>0.16404931726907632</v>
       </c>
       <c r="B188" s="0">
-        <v>0.020045421289494769</v>
+        <v>0.017239523776832362</v>
       </c>
       <c r="C188" s="0">
-        <v>1.4251198081399468</v>
+        <v>1.1712701280009714</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0">
-        <v>0.18026859437751003</v>
+        <v>0.16492658634538152</v>
       </c>
       <c r="B189" s="0">
-        <v>0.019145340378242136</v>
+        <v>0.016798483301277912</v>
       </c>
       <c r="C189" s="0">
-        <v>1.3000114698923837</v>
+        <v>1.1121072748644763</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0">
-        <v>0.18122746987951807</v>
+        <v>0.16580385542168674</v>
       </c>
       <c r="B190" s="0">
-        <v>0.018437059540459856</v>
+        <v>0.016457056684091087</v>
       </c>
       <c r="C190" s="0">
-        <v>1.2056029906054122</v>
+        <v>1.0673598634509929</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0">
-        <v>0.18218634538152612</v>
+        <v>0.16668112449799197</v>
       </c>
       <c r="B191" s="0">
-        <v>0.01788421113480837</v>
+        <v>0.016204912278723324</v>
       </c>
       <c r="C191" s="0">
-        <v>1.1343852657709359</v>
+        <v>1.0349036212264258</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0">
-        <v>0.18314522088353416</v>
+        <v>0.16755839357429719</v>
       </c>
       <c r="B192" s="0">
-        <v>0.017459591057383601</v>
+        <v>0.01603532814974297</v>
       </c>
       <c r="C192" s="0">
-        <v>1.0811579220710357</v>
+        <v>1.0133564623106308</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0">
-        <v>0.18410409638554218</v>
+        <v>0.16843566265060242</v>
       </c>
       <c r="B193" s="0">
-        <v>0.017146522161506472</v>
+        <v>0.015944161838408015</v>
       </c>
       <c r="C193" s="0">
-        <v>1.0427329335771689</v>
+        <v>1.0018666627031871</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0">
-        <v>0.18506297188755019</v>
+        <v>0.16931293172690765</v>
       </c>
       <c r="B194" s="0">
-        <v>0.016934537564160419</v>
+        <v>0.015929301453550742</v>
       </c>
       <c r="C194" s="0">
-        <v>1.0171094367669416</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0">
-        <v>0.18602184738955824</v>
+        <v>0.17019020080321284</v>
       </c>
       <c r="B195" s="0">
-        <v>0.016817290602423818</v>
+        <v>0.015990410023237825</v>
       </c>
       <c r="C195" s="0">
-        <v>1.0030741949672455</v>
+        <v>1.0076871899665227</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0">
-        <v>0.18698072289156625</v>
+        <v>0.17106746987951807</v>
       </c>
       <c r="B196" s="0">
-        <v>0.016791500235609228</v>
+        <v>0.01612888618208877</v>
       </c>
       <c r="C196" s="0">
-        <v>1</v>
+        <v>1.0252158035231778</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0">
-        <v>0.1879395983935743</v>
+        <v>0.1719447389558233</v>
       </c>
       <c r="B197" s="0">
-        <v>0.016856465345219639</v>
+        <v>0.016332975425408</v>
       </c>
       <c r="C197" s="0">
-        <v>1.0077528251044863</v>
+        <v>1.0513253949065233</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0">
-        <v>0.18889847389558231</v>
+        <v>0.17282200803212852</v>
       </c>
       <c r="B198" s="0">
-        <v>0.017013966048167781</v>
+        <v>0.016543589096626718</v>
       </c>
       <c r="C198" s="0">
-        <v>1.0266729598387934</v>
+        <v>1.0786138861908896</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0">
-        <v>0.18985734939759036</v>
+        <v>0.17369927710843375</v>
       </c>
       <c r="B199" s="0">
-        <v>0.017240912327645009</v>
+        <v>0.016754202767845436</v>
       </c>
       <c r="C199" s="0">
-        <v>1.0542448473181347</v>
+        <v>1.1062520082481162</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0">
-        <v>0.1908162248995984</v>
+        <v>0.17457654618473897</v>
       </c>
       <c r="B200" s="0">
-        <v>0.01747111796827942</v>
+        <v>0.016964816439064154</v>
       </c>
       <c r="C200" s="0">
-        <v>1.0825859652439427</v>
+        <v>1.1342397610782034</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0">
-        <v>0.19177510040160645</v>
+        <v>0.1754538152610442</v>
       </c>
       <c r="B201" s="0">
-        <v>0.017701323608913837</v>
+        <v>0.017175430110282872</v>
       </c>
       <c r="C201" s="0">
-        <v>1.1113029923374258</v>
+        <v>1.1625771446811515</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0">
-        <v>0.19273397590361446</v>
+        <v>0.17633108433734937</v>
       </c>
       <c r="B202" s="0">
-        <v>0.017931529249548241</v>
+        <v>0.017386043781501576</v>
       </c>
       <c r="C202" s="0">
-        <v>1.140395928598581</v>
+        <v>1.1912641590569579</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0">
-        <v>0.19369285140562251</v>
+        <v>0.1772083534136546</v>
       </c>
       <c r="B203" s="0">
-        <v>0.018161734890182659</v>
+        <v>0.017596657452720294</v>
       </c>
       <c r="C203" s="0">
-        <v>1.1698647740274113</v>
+        <v>1.2203008042056269</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0">
-        <v>0.19465172690763052</v>
+        <v>0.17808562248995982</v>
       </c>
       <c r="B204" s="0">
-        <v>0.018391940530817063</v>
+        <v>0.017807271123939011</v>
       </c>
       <c r="C204" s="0">
-        <v>1.1997095286239143</v>
+        <v>1.2496870801271571</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0">
-        <v>0.19561060240963854</v>
+        <v>0.17896289156626505</v>
       </c>
       <c r="B205" s="0">
-        <v>0.018622146171451474</v>
+        <v>0.018017884795157729</v>
       </c>
       <c r="C205" s="0">
-        <v>1.2299301923880921</v>
+        <v>1.2794229868215472</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0">
-        <v>0.19656947791164659</v>
+        <v>0.17984016064257027</v>
       </c>
       <c r="B206" s="0">
-        <v>0.018852351812085891</v>
+        <v>0.018228498466376447</v>
       </c>
       <c r="C206" s="0">
-        <v>1.2605267653199448</v>
+        <v>1.3095085242887981</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0">
-        <v>0.1975283534136546</v>
+        <v>0.1807174297188755</v>
       </c>
       <c r="B207" s="0">
-        <v>0.019082557452720295</v>
+        <v>0.018439112137595165</v>
       </c>
       <c r="C207" s="0">
-        <v>1.2914992474194693</v>
+        <v>1.3399436925289099</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0">
-        <v>0.19848722891566265</v>
+        <v>0.1815946987951807</v>
       </c>
       <c r="B208" s="0">
-        <v>0.019312763093354713</v>
+        <v>0.018649725808813876</v>
       </c>
       <c r="C208" s="0">
-        <v>1.3228476386866694</v>
+        <v>1.3707284915418809</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0">
-        <v>0.19944610441767069</v>
+        <v>0.18247196787148592</v>
       </c>
       <c r="B209" s="0">
-        <v>0.019542968733989124</v>
+        <v>0.018860339480032594</v>
       </c>
       <c r="C209" s="0">
-        <v>1.3545719391215427</v>
+        <v>1.4018629213277134</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0">
-        <v>0.20040497991967873</v>
+        <v>0.18334923694779115</v>
       </c>
       <c r="B210" s="0">
-        <v>0.019773174374623542</v>
+        <v>0.019070953151251312</v>
       </c>
       <c r="C210" s="0">
-        <v>1.3866721487240912</v>
+        <v>1.4333469818864071</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0">
-        <v>0.20136385542168675</v>
+        <v>0.18422650602409638</v>
       </c>
       <c r="B211" s="0">
-        <v>0.020003380015257945</v>
+        <v>0.019281566822470037</v>
       </c>
       <c r="C211" s="0">
-        <v>1.4191482674943112</v>
+        <v>1.465180673217962</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0">
-        <v>0.20232273092369479</v>
+        <v>0.1851037751004016</v>
       </c>
       <c r="B212" s="0">
-        <v>0.020233585655892363</v>
+        <v>0.019492180493688754</v>
       </c>
       <c r="C212" s="0">
-        <v>1.4520002954322069</v>
+        <v>1.4973639953223763</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0">
-        <v>0.20328160642570281</v>
+        <v>0.18598104417670683</v>
       </c>
       <c r="B213" s="0">
-        <v>0.020463791296526767</v>
+        <v>0.019702794164907472</v>
       </c>
       <c r="C213" s="0">
-        <v>1.4852282325377748</v>
+        <v>1.5298969481996521</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0">
-        <v>0.20424048192771083</v>
+        <v>0.18685831325301205</v>
       </c>
       <c r="B214" s="0">
-        <v>0.020693996937161178</v>
+        <v>0.01991340783612619</v>
       </c>
       <c r="C214" s="0">
-        <v>1.5188320788110179</v>
+        <v>1.5627795318497877</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0">
-        <v>0.20519935742971887</v>
+        <v>0.18773558232931725</v>
       </c>
       <c r="B215" s="0">
-        <v>0.020924202577795596</v>
+        <v>0.020124021507344901</v>
       </c>
       <c r="C215" s="0">
-        <v>1.5528118342519357</v>
+        <v>1.5960117462727827</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0">
-        <v>0.20615823293172689</v>
+        <v>0.18861285140562248</v>
       </c>
       <c r="B216" s="0">
-        <v>0.021154408218429999</v>
+        <v>0.020334635178563619</v>
       </c>
       <c r="C216" s="0">
-        <v>1.5871674988605253</v>
+        <v>1.6295935914686401</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0">
-        <v>0.20711710843373493</v>
+        <v>0.18949012048192771</v>
       </c>
       <c r="B217" s="0">
-        <v>0.021384613859064417</v>
+        <v>0.020545248849782337</v>
       </c>
       <c r="C217" s="0">
-        <v>1.6218990726367906</v>
+        <v>1.6635250674373576</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0">
-        <v>0.20807598393574298</v>
+        <v>0.19036738955823293</v>
       </c>
       <c r="B218" s="0">
-        <v>0.021614819499698828</v>
+        <v>0.020755862521001055</v>
       </c>
       <c r="C218" s="0">
-        <v>1.657006555580729</v>
+        <v>1.6978061741789357</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0">
-        <v>0.20903485943775102</v>
+        <v>0.19124465863453816</v>
       </c>
       <c r="B219" s="0">
-        <v>0.021845025140333246</v>
+        <v>0.020966476192219773</v>
       </c>
       <c r="C219" s="0">
-        <v>1.6924899476923425</v>
+        <v>1.7324369116933749</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0">
-        <v>0.20999373493975904</v>
+        <v>0.19212192771084338</v>
       </c>
       <c r="B220" s="0">
-        <v>0.022075230780967649</v>
+        <v>0.02117708986343849</v>
       </c>
       <c r="C220" s="0">
-        <v>1.7283492489716277</v>
+        <v>1.767417279980674</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0">
-        <v>0.21095261044176708</v>
+        <v>0.19299919678714858</v>
       </c>
       <c r="B221" s="0">
-        <v>0.022305436421602067</v>
+        <v>0.021387703534657201</v>
       </c>
       <c r="C221" s="0">
-        <v>1.7645844594185887</v>
+        <v>1.8027472790408328</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0">
-        <v>0.2119114859437751</v>
+        <v>0.19387646586345381</v>
       </c>
       <c r="B222" s="0">
-        <v>0.022535642062236471</v>
+        <v>0.021598317205875919</v>
       </c>
       <c r="C222" s="0">
-        <v>1.8011955790332215</v>
+        <v>1.8384269088738538</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0">
-        <v>0.21287036144578314</v>
+        <v>0.19475373493975903</v>
       </c>
       <c r="B223" s="0">
-        <v>0.022765847702870889</v>
+        <v>0.021808930877094637</v>
       </c>
       <c r="C223" s="0">
-        <v>1.8381826078155308</v>
+        <v>1.8744561694797348</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0">
-        <v>0.21382923694779116</v>
+        <v>0.19563100401606426</v>
       </c>
       <c r="B224" s="0">
-        <v>0.0229960533435053</v>
+        <v>0.022019544548313355</v>
       </c>
       <c r="C224" s="0">
-        <v>1.8755455457655126</v>
+        <v>1.9108350608584765</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0">
-        <v>0.21478811244979917</v>
+        <v>0.19650827309236948</v>
       </c>
       <c r="B225" s="0">
-        <v>0.023226258984139703</v>
+        <v>0.022230158219532073</v>
       </c>
       <c r="C225" s="0">
-        <v>1.9132843928831667</v>
+        <v>1.9475635830100795</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0">
-        <v>0.21574698795180722</v>
+        <v>0.19738554216867471</v>
       </c>
       <c r="B226" s="0">
-        <v>0.023456464624774121</v>
+        <v>0.022440771890750791</v>
       </c>
       <c r="C226" s="0">
-        <v>1.9513991491684977</v>
+        <v>1.9846417359345423</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0">
-        <v>0.21670586345381526</v>
+        <v>0.19826281124497994</v>
       </c>
       <c r="B227" s="0">
-        <v>0.023686670265408532</v>
+        <v>0.022651385561969516</v>
       </c>
       <c r="C227" s="0">
-        <v>1.9898898146215012</v>
+        <v>2.022069519631867</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0">
-        <v>0.21766473895582331</v>
+        <v>0.19914008032128513</v>
       </c>
       <c r="B228" s="0">
-        <v>0.02391687590604295</v>
+        <v>0.022861999233188227</v>
       </c>
       <c r="C228" s="0">
-        <v>2.0287563892421798</v>
+        <v>2.0598469341020507</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0">
-        <v>0.21862361445783132</v>
+        <v>0.20001734939759036</v>
       </c>
       <c r="B229" s="0">
-        <v>0.024147081546677354</v>
+        <v>0.023072612904406944</v>
       </c>
       <c r="C229" s="0">
-        <v>2.0679988730305294</v>
+        <v>2.0979739793450953</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0">
-        <v>0.21958248995983937</v>
+        <v>0.20089461847389559</v>
       </c>
       <c r="B230" s="0">
-        <v>0.024377287187311771</v>
+        <v>0.023283226575625662</v>
       </c>
       <c r="C230" s="0">
-        <v>2.1076172659865562</v>
+        <v>2.1364506553610005</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0">
-        <v>0.22054136546184738</v>
+        <v>0.20177188755020081</v>
       </c>
       <c r="B231" s="0">
-        <v>0.024607492827946182</v>
+        <v>0.02349384024684438</v>
       </c>
       <c r="C231" s="0">
-        <v>2.1476115681102557</v>
+        <v>2.1752769621497672</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0">
-        <v>0.22150024096385543</v>
+        <v>0.20264915662650604</v>
       </c>
       <c r="B232" s="0">
-        <v>0.024837698468580593</v>
+        <v>0.023704453918063098</v>
       </c>
       <c r="C232" s="0">
-        <v>2.1879817794016288</v>
+        <v>2.2144528997113935</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0">
-        <v>0.22245911646586344</v>
+        <v>0.20352642570281124</v>
       </c>
       <c r="B233" s="0">
-        <v>0.025067904109215004</v>
+        <v>0.023915067589281809</v>
       </c>
       <c r="C233" s="0">
-        <v>2.228727899860675</v>
+        <v>2.2539784680458794</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0">
-        <v>0.22341799196787149</v>
+        <v>0.20440369477911646</v>
       </c>
       <c r="B234" s="0">
-        <v>0.025298109749849414</v>
+        <v>0.024125681260500527</v>
       </c>
       <c r="C234" s="0">
-        <v>2.2698499294873957</v>
+        <v>2.2938536671532277</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0">
-        <v>0.22437686746987953</v>
+        <v>0.20528096385542166</v>
       </c>
       <c r="B235" s="0">
-        <v>0.025528315390483832</v>
+        <v>0.024336294931719238</v>
       </c>
       <c r="C235" s="0">
-        <v>2.3113478682817923</v>
+        <v>2.3340784970334347</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0">
-        <v>0.22533574297188755</v>
+        <v>0.20615823293172689</v>
       </c>
       <c r="B236" s="0">
-        <v>0.025758521031118236</v>
+        <v>0.024546908602937956</v>
       </c>
       <c r="C236" s="0">
-        <v>2.3532217162438593</v>
+        <v>2.3746529576865045</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0">
-        <v>0.22629461847389559</v>
+        <v>0.20703550200803211</v>
       </c>
       <c r="B237" s="0">
-        <v>0.025988726671752654</v>
+        <v>0.024757522274156674</v>
       </c>
       <c r="C237" s="0">
-        <v>2.3954714733736027</v>
+        <v>2.415577049112434</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0">
-        <v>0.22725349397590361</v>
+        <v>0.20791277108433734</v>
       </c>
       <c r="B238" s="0">
-        <v>0.026218932312387058</v>
+        <v>0.024968135945375392</v>
       </c>
       <c r="C238" s="0">
-        <v>2.4380971396710178</v>
+        <v>2.456850771311224</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0">
-        <v>0.22821236947791165</v>
+        <v>0.20879004016064256</v>
       </c>
       <c r="B239" s="0">
-        <v>0.026449137953021475</v>
+        <v>0.025178749616594109</v>
       </c>
       <c r="C239" s="0">
-        <v>2.4810987151361097</v>
+        <v>2.4984741242828754</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0">
-        <v>0.22917124497991967</v>
+        <v>0.20966730923694779</v>
       </c>
       <c r="B240" s="0">
-        <v>0.026679343593655886</v>
+        <v>0.025389363287812827</v>
       </c>
       <c r="C240" s="0">
-        <v>2.5244761997688743</v>
+        <v>2.5404471080273869</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0">
-        <v>0.23013012048192771</v>
+        <v>0.21054457831325299</v>
       </c>
       <c r="B241" s="0">
-        <v>0.026909549234290297</v>
+        <v>0.025599976959031538</v>
       </c>
       <c r="C241" s="0">
-        <v>2.5682295935693116</v>
+        <v>2.5827697225447572</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0">
-        <v>0.23108899598393573</v>
+        <v>0.21142184738955822</v>
       </c>
       <c r="B242" s="0">
-        <v>0.027139754874924708</v>
+        <v>0.025810590630250263</v>
       </c>
       <c r="C242" s="0">
-        <v>2.6123588965374238</v>
+        <v>2.6254419678349912</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0">
-        <v>0.23204787148594378</v>
+        <v>0.21229911646586344</v>
       </c>
       <c r="B243" s="0">
-        <v>0.027369960515559119</v>
+        <v>0.026021204301468981</v>
       </c>
       <c r="C243" s="0">
-        <v>2.6568641086732101</v>
+        <v>2.6684638438980852</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0">
-        <v>0.23300674698795182</v>
+        <v>0.21317638554216867</v>
       </c>
       <c r="B244" s="0">
-        <v>0.027600166156193536</v>
+        <v>0.026231817972687699</v>
       </c>
       <c r="C244" s="0">
-        <v>2.7017452299766713</v>
+        <v>2.7118353507340389</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0">
-        <v>0.23396562248995986</v>
+        <v>0.21405365461847389</v>
       </c>
       <c r="B245" s="0">
-        <v>0.027830371796827947</v>
+        <v>0.026442431643906417</v>
       </c>
       <c r="C245" s="0">
-        <v>2.7470022604478044</v>
+        <v>2.7555564883428536</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0">
-        <v>0.23492449799196788</v>
+        <v>0.21493092369477912</v>
       </c>
       <c r="B246" s="0">
-        <v>0.028060577437462358</v>
+        <v>0.026653045315125135</v>
       </c>
       <c r="C246" s="0">
-        <v>2.7926352000866124</v>
+        <v>2.7996272567245293</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0">
-        <v>0.2358833734939759</v>
+        <v>0.21580819277108435</v>
       </c>
       <c r="B247" s="0">
-        <v>0.028290783078096762</v>
+        <v>0.026863658986343853</v>
       </c>
       <c r="C247" s="0">
-        <v>2.8386440488930926</v>
+        <v>2.8440476558790646</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0">
-        <v>0.23684224899598394</v>
+        <v>0.21668546184738954</v>
       </c>
       <c r="B248" s="0">
-        <v>0.028520988718731179</v>
+        <v>0.027074272657562563</v>
       </c>
       <c r="C248" s="0">
-        <v>2.8850288068672496</v>
+        <v>2.88881768580646</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0">
-        <v>0.23780112449799196</v>
+        <v>0.21756273092369477</v>
       </c>
       <c r="B249" s="0">
-        <v>0.02875119435936559</v>
+        <v>0.027284886328781281</v>
       </c>
       <c r="C249" s="0">
-        <v>2.9317894740090789</v>
+        <v>2.9339373465067169</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0">
-        <v>0.23876</v>
+        <v>0.21844</v>
       </c>
       <c r="B250" s="0">
-        <v>0.028981400000000001</v>
+        <v>0.027495499999999999</v>
       </c>
       <c r="C250" s="0">
-        <v>2.9789260503185817</v>
+        <v>2.9794066379798343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>